<commit_message>
more narratives in, still some missing
</commit_message>
<xml_diff>
--- a/excel_books/narratives_tables.xlsx
+++ b/excel_books/narratives_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n740789\Documents\sfdr_report_generator\excel_books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84E2290-B391-47AA-8543-0EC2B8CC468C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B2F092-7B03-4CFE-9D83-82FCB8A1924C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17475" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{876AE5F7-9A61-4241-A259-03591D994349}"/>
+    <workbookView xWindow="15855" yWindow="-16440" windowWidth="29040" windowHeight="16440" xr2:uid="{876AE5F7-9A61-4241-A259-03591D994349}"/>
   </bookViews>
   <sheets>
     <sheet name="spanish" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5927" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5927" uniqueCount="241">
   <si>
     <t>macro_narrative</t>
   </si>
@@ -1227,16 +1227,6 @@
                 &lt;p&gt;En el caso en el que el Plan de Previsión haya invertido en IICs de terceras partes, la Gestora utilizó la metodología de no causar daño significativo divulgada por las gestoras terceras.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Para garantizar que la contribución positiva a un objetivo de inversión sostenible medioambiental o social no ha causado un perjuicio significativo a otros objetivos sostenibles durante el periodo de referencia, la Entidad contratada para la gestión de activos de la EPSV ha aplicado las siguientes salvaguardas basadas en su metodología interna con el fin de demostrar que existe la intención de no causar un daño:&lt;/p&gt;
-                &lt;ul&gt;
-                    &lt;li&gt;Consideración de los indicadores obligatorios de incidencias adversas en materia de sostenibilidad (PIAS) recogidos en el anexo I del Reglamento Delegado (UE) 2022/1288/97, por el que se completa el Reglamento (UE) 2019/2088, tal cual como se describe en la siguiente pregunta.&lt;/li&gt;
-                    &lt;li&gt;Actividad en sectores controvertidos: mediante el análisis y exclusión de emisores con exposiciones significativas a actividades controvertidas en sectores como combustibles fósiles, armas controvertidas, tabaco, entre otros, así como controversias expuestas a controversias severas.&lt;/li&gt;
-                    &lt;li&gt;Desempeño sostenible neutro: la Gestora ha requerido una calificación ASG mínima de B en una escala de 7 niveles (C-, C, C+, B, A-, A y A+, donde A+ refleja el mejor desempeño ASG) de acuerdo con su metodología propia para garantizar que las prácticas de sostenibilidad de cada emisor cumplen con unos requisitos ASG mínimos.&lt;/li&gt;
-                &lt;/ul&gt;
-                &lt;p&gt;Si alguna inversión directa del Fondo ha incumplido con alguna de estas salvaguardas, la Gestora ha considerado que no es posible asegurar que haya existido un daño significativo y no se ha considerado como inversión sostenible&lt;/p&gt;
-                &lt;p&gt;En el caso en el que el Plan de Previsión haya invertido en IICs de terceras partes, la Gestora utilizó la metodología de no causar daño significativo divulgada por las gestoras terceras.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;La Entidad contratada para la gestión de activos de la EPSV ha tenido en cuenta ha tenido en consideración los indicadores obligatorios de principales incidencias adversas en el análisis del principio de no causar daño significativo de los subyacentes de este Plan de Previsión.&lt;/p&gt;
 &lt;p&gt;Para ello, la Entidad contratada para la gestión de activos de la EPSV ha definido umbrales basados en criterios cuantitativos y cualitativos, siendo estos:&lt;/p&gt;
 &lt;ul&gt;
@@ -1391,6 +1381,197 @@
   </si>
   <si>
     <t>&lt;div class="sub-qtext"&gt;¿Cómo difiere el índice de referencia de un índice general de mercado?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt; Con respecto al periodo de referencia anterior, el rendimiento de los indicadores de sostenibilidad ha sido:&lt;/p&gt;
+&lt;ul&gt; 
+&lt;li&gt;Indicador de exclusiones: Se ha mantenido en 0%. &lt;/li&gt;
+&lt;li&gt; Indicador de controversias: Se ha mantenido en 0%. &lt;/li&gt;
+&lt;li&gt;Calificación/Rating ASG mínimo medio del Fondo: En {{YEAR_PREV}} este indicador fue {{ESG_RATING_23}} y en {{YEAR}} ha sido {{ESG_RATING_24}}. &lt;/li&gt;
+&lt;li&gt; El porcentaje medio de activos subyacentes del Fondo alineados con las características medioambientales y sociales promovidas ha sido en ambos periodos de referencia de al menos el 51%&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Con respecto al periodo de referencia anterior, el rendimiento de los indicadores de sostenibilidad ha sido:&lt;/p&gt;
+&lt;ul&gt; 
+&lt;li&gt;Indicador de exclusiones: Se ha mantenido en 0%. &lt;/li&gt;
+&lt;li&gt; Indicador de controversias: Se ha mantenido en 0%. &lt;/li&gt;
+&lt;li&gt;Calificación/Rating ASG mínimo medio del Fondo: En {{YEAR_PREV}} este indicador fue {{ESG_RATING_23}} y en {{YEAR}} ha sido {{ESG_RATING_24}}. &lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Las &lt;strong&gt;actividades facilitadoras&lt;/strong&gt;  permiten de forma directa que otras actividades contribuyan significativamente a un objetivo medioambiental.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;El Plan de Previsión no tiene establecido un porcentaje mínimo de alineamiento de las inversiones de este Plan de Previsión a la Taxonomía de la UE. El porcentaje de inversiones alineadas con la Taxonomía de la UE en comparación con el período de referencia anterior ha {{ENCREASE_DECREASE_EUTAXO_ALIGNMENT}}.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;El Fondos no tiene establecido un porcentaje mínimo de alineamiento de las inversiones de este Plan de Previsión a la Taxonomía de la UE. El porcentaje de inversiones alineadas con la Taxonomía de la UE en comparación con el período de referencia anterior ha {{ENCREASE_DECREASE_EUTAXO_ALIGNMENT}}.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;¿De qué manera las inversiones sostenibles que el producto financiero ha realizado en parte no causan un perjuicio significativo a ningún objetivo de inversión sostenible medioambiental o social?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Para garantizar que la contribución positiva a un objetivo de inversión sostenible medioambiental o social no ha causado un perjuicio significativo a otros objetivos sostenibles durante el periodo de referencia, la Entidad contratada para la gestión de activos de la EPSV ha aplicado las siguientes salvaguardas basadas en su metodología interna con el fin de demostrar que existe la intención de no causar un daño:&lt;/p&gt;                
+&lt;ul&gt;
+&lt;li&gt;Consideración de los indicadores obligatorios de incidencias adversas en materia de sostenibilidad (PIAS) recogidos en el anexo I del Reglamento Delegado (UE) 2022/1288/97, por el que se completa el Reglamento (UE) 2019/2088, tal cual como se describe en la siguiente pregunta.&lt;/li&gt;
+&lt;li&gt;Actividad en sectores controvertidos: mediante el análisis y exclusión de emisores con exposiciones significativas a actividades controvertidas en sectores como combustibles fósiles, armas controvertidas, tabaco, entre otros, así como controversias expuestas a controversias severas.&lt;/li&gt;
+&lt;li&gt;Desempeño sostenible neutro: la Gestora ha requerido una calificación ASG mínima de B en una escala de 7 niveles (C-, C, C+, B, A-, A y A+, donde A+ refleja el mejor desempeño ASG) de acuerdo con su metodología propia para garantizar que las prácticas de sostenibilidad de cada emisor cumplen con unos requisitos ASG mínimos.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Si alguna inversión directa del Fondo ha incumplido con alguna de estas salvaguardas, la Gestora ha considerado que no es posible asegurar que haya existido un daño significativo y no se ha considerado como inversión sostenible&lt;/p&gt;
+&lt;p&gt;En el caso en el que el Plan de Previsión haya invertido en IICs de terceras partes, la Gestora utilizó la metodología de no causar daño significativo divulgada por las gestoras terceras.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;El Fondo ha tenido una proporción del {{OTHERS}}% del patrimonio del Fondo a lo largo del periodo de referencia a inversiones que no están alineadas con las características medioambientales y sociales promovidas por el Fondo. Este porcentaje ha sido calculado como el porcentaje medio del Fondo teniendo en cuenta las inversiones subyacentes del último día hábil de cada trimestre del período de referencia, tal como se define en la sección Inversiones principales.&lt;/p&gt;
+&lt;p style="margin-top: -10px;"&gt;                   
+Estas inversiones no alteraron el logro de las características medioambientales y sociales promovidas por el Fondo, y su propósito ha sido el de contribuir a la gestión eficiente de la cartera, proporcionar liquidez y un propósito de cobertura. &lt;/p&gt;
+&lt;p style="margin-top: -10px;"&gt; La Gestora ha establecido salvaguardias ambientales o sociales  mínimas para no causar un perjuicio significativo, como la consideración de los principales incidencias adversas, o la exclusión de actividades no alineadas con las características ambientales y/o sociales del Fondo. Los activos que podían considerarse eran los siguientes:&lt;/p&gt;
+&lt;ul&gt;
+                    &lt;li&gt;Activos de inversión directa de contado que no dispusieran de calificación / rating ASG por falta de datos del proveedor utilizado por la Gestora y que no puedan ser consideradas inversiones sostenibles. Estos activos cumplen los criterios de exclusión del Fondo, asegurando así unas salvaguardas mínimas.&lt;/li&gt;
+                    &lt;li&gt;IIC que no dispusieran de calificación / rating ASG por falta de datos y que no puedan ser clasificadas como IIC del art. 8 o 9 del Reglamento (UE) 2019/2088. Dentro de los procedimientos de selección de IIC se aplican unas salvaguardas mínimas siempre que esté de acuerdo con el procedimiento interno de la Gestora.&lt;/li&gt;
+                    &lt;li&gt;Otros activos de contado distintos de los señalados anteriormente (i.e.: ETC) que estén permitidos por la política del Fondo y para los que se aplican unas salvaguardas mínimas.&lt;/li&gt;
+                    &lt;li&gt;Liquidez en el depositario y resto de cuentas corrientes utilizadas para la operativa ordinaria del Fondo (i.e.: garantías de derivados, etc.).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Adicionalmente, para las inversiones en instrumentos financieros derivados no les resulta de aplicación los procedimientos descritos para la promoción de las características ASG.&lt;/p&gt;
+&lt;p style="margin-top: -10px;"&gt;En este caso la Gestora tiene establecido procedimientos para verificar que dichos instrumentos no alteran la consecución de las características ambientales o sociales promovidas por el Fondo, pudiendo utilizarse dichos instrumentos con la finalidad de cobertura y de gestión eficiente de la cartera del Fondo de inversión como elemento diversificador y de gestión.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt; Durante el período de referencia, se han adoptado las siguientes medidas para cumplir con las características medioambientales y sociales del Fondo : &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;La Gestora ha revisado periódicamente que el Fondo ha cumplido con las siguientes exclusiones.
+&lt;ul&gt;
+&lt;li&gt;Se han excluido emisores con exposición (medida en términos de volumen de negocios) relacionada con armas controvertidas, y/o con una exposición significativa a combustibles fósiles no convencionales y/o actividades la generación eléctrica a partir del carbón y/o la minería de carbón. &lt;/li&gt;
+&lt;li&gt;Se han excluido del universo de inversiones aquellos emisores en los que se han identificado controversias consideradas críticas en materia medioambiental, social o de gobernanza.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;La Gestora ha supervisado periódicamente que la calificación / rating ASG mínima medio de los emisores de los activos de la cartera de inversión directa de contado e IIC con rating del Fondo ha sido de al menos A-, de acuerdo con la metodología propia de la Gestora en una escala de 7 niveles (C-, C, C+, B, A-, A y A+, donde A+ refleja el mejor desempeño ASG).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Adicionalmente, la Gestora también consideró que los siguientes casos también cumplían con las características medioambientales y sociales promovidas por el Fondo, y se contabilizaban como tal:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Los casos de un emisor sin calificación ASG o que no cumpliera con los indicadores ASG establecidos en la estrategia de inversión, pero que tengan inversiones que puedan ser consideradas inversiones sostenibles, y en concreto emisiones de dicho emisor que puedan ser calificadas como bono verde, social o sostenible, estas emisiones podrían formar parte del universo de activos que promueven las características ASG del Fondo, tras la validación previa de la Gestora, de conformidad con su metodología de análisis propia. &lt;/li&gt;
+&lt;li&gt;Las IICs que, aunque no tengan asignado un rating ASG por la Gestora, sean IICs que promuevan características ASG. (IIC consideradas art. 8 Reglamento (UE) 2019/2088 y/o que tengan como objetivo inversiones sostenibles (art. 9 conforme con el Reglamento (UE) 2019/2088)).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Los criterios ASG anteriores, junto con el cumplimiento de los compromisos mínimos del Fondo se integraron en el proceso de inversión y fueron supervisados periódicamente por el equipo de Cumplimiento de la Gestora. En caso de incumplimiento, se tomaron las medidas correctivas necesarias (por ejemplo, comunicación con el equipo SRI, remisión al comité correspondiente, entre otros).&lt;/p&gt;
+&lt;p&gt;Además,el desempeño ASG de los emisores ha sido objeto de un seguimiento sistemático y continuo por parte del equipo SRI de la Gestora, incluido el seguimiento continuo de las posibles discrepancias detectadas por los gestores y los datos del modelo proporcionado por los proveedores.&lt;/p&gt;
+&lt;p&gt;Por último, la Gestora ha llevado a cabo actividades de engagement con emisores privados y actividades de voto en los casos en que el tipo de activo lo permite (acciones). Estas actividades estaban alineadas con las características sociales y medioambientales del Fondo y con las Políticas de Engagement y Voto de la Gestora disponibles en https://www.santanderassetmanagement.es/sostenibilidad/. Para ver más ejemplos de las actividades de engagement y voto realizadas, se puede consultar el informe de implicación y voto de la Gestora disponible en: https://www.santanderassetmanagement.es/sostenibilidad/&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;La &lt;strong&gt;taxonomía de la UE&lt;/strong&gt; es un sistema de clasificación previsto en el Reglamento (UE) 2020/852 por el que se establece una lista de &lt;strong&gt;actividades económicas medioambientalmente sostenibles.&lt;/strong&gt; Dicho Reglamento no incluye una lista de actividades económicas socialmente sostenibles. Las inversiones sostenibles con un objetivo medioambiental pueden ajustarse, o no, a la taxonomía. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;El Fondo ha promovido características medioambientales y sociales evaluando sus inversiones subyacentes en función de criterios ambientales, sociales y de gobernanza (ASG) utilizando una metodología ASG propia e invirtiendo en emisores que exhiban prácticas ASG sólidas y cumplan con los factores de exclusión descritos en la estrategia de inversión recogida en el anexo de Sostenibilidad de la información precontractual de este Fondo.&lt;/p&gt;
+&lt;p&gt;En este sentido, se han utilizado elementos financieros, ambientales, sociales y de buen gobierno para obtener una visión más completa de los activos subyacentes en los que el Fondo invirtió durante el período de referencia, habiendo evaluado una combinación de factores ASG que incluyeron, pero no se limitaron a:&lt;/p&gt;
+    &lt;ul&gt;
+        &lt;li&gt;Factores ambientales mediante la evaluación del desempeño cuantitativo y cualitativo de los emisores en asuntos como las emisiones de gases de efecto invernadero, el agotamiento de recursos, la contaminación y la gestión del agua. Estos factores han sido aplicables tanto a emisores públicos como privados. Por la parte de deuda pública, se valoraron factores específicos como políticas y gastos en educación y salud, empleo, calidad social, compromiso con diferentes convenciones relativas a derechos humanos y laborales, entre otros. &lt;/li&gt;
+        &lt;li&gt;Factores sociales abarcando desde cuestiones relacionadas con el lugar de trabajo, el cumplimiento de los estándares laborales o la gestión del talento, hasta las relaciones con las comunidades locales, la privacidad y la seguridad de los datos y los derechos humanos. &lt;/li&gt;
+        &lt;li&gt;Factores de gobernanza incluyendo la calidad de la gestión de un emisor, su cultura y ética, la eficacia de los sistemas de gobernanza para minimizar el riesgo de mala gestión y la capacidad para anticipar los riesgos operativos y legales que podrían representar un incumplimiento. También se han considerado factores relacionados con la composición y estructura del consejo del emisor. Por la parte de deuda pública, se valoraron factores específicos como son calidad regulatoria y de las leyes de los Estados, control de la corrupción, gastos en I+D, entre otros. &lt;/li&gt;
+    &lt;/ul&gt;
+&lt;p&gt;La evaluación de estos factores para cada emisor se basó en la materialidad sectorial definida por la Gestora como parte de su metodología ASG. De manera adicional a estos factores, los casos de controversias también fueron evaluados considerando la gravedad de su impacto en la sociedad, el medioambiente y el impacto en los grupos de interés y, en consecuencia, se integraron dentro de la metodología ASG de la Gestora. &lt;/p&gt;
+&lt;p&gt;La Gestora también promovió características medioambientales y sociales mediante la aplicación de acciones de engagement, ya sea individualmente o mediante iniciativas colaborativas, para promover mejores prácticas ASG de acuerdo con su política de engagement.&lt;p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;¿Cómo se han comportado los indicadores de sostenibilidad?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; A continuación, se describe el comportamiento de los indicadores de sostenibilidad del Fondo a lo largo del período de referencia:&lt;/p&gt;
+&lt;ul&gt; 
+&lt;li&gt; &lt;strong&gt;Indicador de exclusiones:&lt;/strong&gt; El Fondo no ha realizado ninguna inversión en sectores no permitidos por la política de inversión del mismo de acuerdo con el procedimiento interno de la Gestora. Es decir, el Fondo no tuvo exposición a activos de inversión directa de contado de emisores, así como los instrumentos financieros derivados (futuros y opciones sobre acciones) utilizados por el Fondo para tomar como referencia el índice en los que el emisor del subyacente de dichos derivados mayoritariamente orientados a actividades relacionadas con el armamento controvertido, así como los combustibles fósiles no convencionales y la generación eléctrica a partir del carbón y minería de carbón. . Adicionalmente, para el caso de la renta fija pública, el Fondo no ha tenido exposición a países con un desempeño deficiente en términos de derechos políticos y libertades sociales. &lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Indicador de controversias:&lt;/strong&gt; El Fondo ha tenido una exposición del 0% a activos de inversión directa de contado de emisores, así como los instrumentos financieros derivados (futuros y opciones sobre acciones) utilizados por el Fondo para tomar como referencia el índice en los que el emisor del subyacente de dichos derivados haya estado involucrado en controversias consideradas críticas.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Calificación/Rating ASG mínimo medio del Fondo:&lt;/strong&gt; La calificación ASG promedio de los emisores de los activos con rating de la cartera de inversión directa de contado e IIC y emisores de los subyacentes de los futuros y opciones sobre acciones utilizados por el Fondo para tomar como referencia el índice con rating según la metodología interna de la Gestora fue {{ESG_RATING_24}} en una escala de 7 niveles (C-, C, C+, B, A-, a y A+, donde A+ refleja el mejor rendimiento ASG). Este valor se ha calculado como la calificación ASG media teniendo en cuenta los datos del último día hábil de cada trimestre del período de referencia.&lt;/li&gt;
+&lt;li&gt;El porcentaje medio de activos subyacentes del Fondo alineados con las características medioambientales y sociales promovidas fue del &lt;strong&gt;{{SFDR_LAST_REP_INV_WITH_ENV_SOC}}%&lt;/strong&gt; a lo largo del periodo de referencia. &lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt; ¿... y en comparación con periodos anteriores?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;¿Cuáles han sido los objetivos de las inversiones sostenibles que ha realizado en parte el producto financiero y de qué forma ha contribuido la inversión sostenible a dichos objetivos?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Los objetivos de inversión sostenible de este Fondo se alcanzaron invirtiendo en emisores que contribuyeron al menos a uno de los objetivos definidos en el Anexo de Sostenibilidad de la información precontractual de este Fondo. En la práctica, los subyacentes que se han contabilizado como inversión sostenible son aquellos emisores que han cumplido al menos uno de los siguientes criterios:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Emisores cuyas actividades están alineadas con la trayectoria de descarbonización en virtud del Acuerdo de París o son actualmente Net Zero. Los emisores que han cumplido con este criterio contribuyeron a alcanzar objetivos medioambientalmente sostenibles, como la mitigación del cambio climático, ayudando a estabilizar las concentraciones de gases de efecto invernadero en la atmósfera y/o la adaptación al cambio climático invirtiendo en soluciones de adaptación que reduzcan o prevengan sustancialmente el riesgo efectos climáticos adversos. &lt;/li&gt;
+&lt;li&gt;Emisores cuyas prácticas están al menos en un 20% en términos de ingresos alineadas con los objetivos de mitigación y/o adaptación de la Taxonomía de la UE. A la fecha del presente documento, se consideró que los emisores que cumplen con este criterio contribuyeron a los objetivos medioambientales de mitigación y/o adaptación al cambio climático descritos anteriormente. &lt;/li&gt;
+&lt;li&gt;Emisores que generan al menos un 20% de ingresos derivados de productos y/o servicios que generan un impacto medioambiental medible (es decir, emisores que desarrollan prácticas agrícolas sostenibles, tecnologías de prevención de la contaminación o energías alternativas, entre otros). Se ha considerado que los emisores que cumplieron con este criterio contribuyeron a objetivos medioambientalmente sostenibles, como la prevención y el control de la contaminación, la protección y recuperación de la biodiversidad y los ecosistemas y el uso sostenible y la protección de los recursos hídricos y marinos. &lt;/li&gt;
+&lt;li&gt;Emisores que generan al menos un 20% de ingresos derivados de productos y/o servicios que generan un impacto social medible (es decir, emisores que desarrollan soluciones educativas, mejora de la conectividad o soluciones de tratamiento de enfermedades, entre otros). Los emisores que cumplieron con este criterio contribuyeron a alcanzar objetivos sociales sostenibles, como estándares de vida adecuados y bienestar de los consumidores, contribuyendo a la creación de productos y servicios que satisfagan las necesidades humanas. 
+&lt;li&gt;Emisores cuyas prácticas corporativas demuestran su intención de contribuir a los objetivos medioambientales y/o sociales sostenibles del Fondo a través de su desempeño líder en sostenibilidad basado en la puntuación ASG de la Gestora. &lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Las inversiones en bonos verdes, bonos sociales, y bonos sostenibles también se consideraron contribuyentes a los objetivos de sostenibilidad medioambiental o social del Fondo mediante la financiación de proyectos verdes, sociales o sostenibles de acuerdo con estándares de referencia como los desarrollados por la Asociación Internacional del Mercado de Capitales (“ICMA”).&lt;/p&gt;
+&lt;p&gt; Cuando el Fondo ha invertido en IICs de terceras partes, la Gestora utilizó los datos y metodologías de inversión sostenible divulgados por las gestoras terceras.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Para garantizar que la contribución positiva a un objetivo de inversión sostenible medioambiental o social no ha causado un perjuicio significativo a otros objetivos sostenibles durante el periodo de referencia, la Entidad contratada para la gestión de activos de la EPSV ha aplicado las siguientes salvaguardas basadas en su metodología interna con el fin de demostrar que existe la intención de no causar un daño:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Consideración de los indicadores obligatorios de incidencias adversas en materia de sostenibilidad (PIAS) recogidos en el anexo I del Reglamento Delegado (UE) 2022/1288/97, por el que se completa el Reglamento (UE) 2019/2088, tal cual como se describe en la siguiente pregunta.&lt;/li&gt;
+&lt;li&gt;Actividad en sectores controvertidos: mediante el análisis y exclusión de emisores con exposiciones significativas a actividades controvertidas en sectores como combustibles fósiles, armas controvertidas, tabaco, entre otros, así como controversias expuestas a controversias severas.&lt;/li&gt;
+&lt;li&gt;Desempeño sostenible neutro: la Gestora ha requerido una calificación ASG mínima de B en una escala de 7 niveles (C-, C, C+, B, A-, A y A+, donde A+ refleja el mejor desempeño ASG) de acuerdo con su metodología propia para garantizar que las prácticas de sostenibilidad de cada emisor cumplen con unos requisitos ASG mínimos.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Si alguna inversión directa del Fondo ha incumplido con alguna de estas salvaguardas, la Gestora ha considerado que no es posible asegurar que haya existido un daño significativo y no se ha considerado como inversión sostenible&lt;/p&gt;
+&lt;p&gt;En el caso en el que el Plan de Previsión haya invertido en IICs de terceras partes, la Gestora utilizó la metodología de no causar daño significativo divulgada por las gestoras terceras.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Para garantizar que la contribución positiva a un objetivo de inversión sostenible medioambiental o social no ha causado un perjuicio significativo a otros objetivos sostenibles durante el periodo de referencia, la Entidad contratada para la gestión de activos de la EPSV ha aplicado las siguientes salvaguardas basadas en su metodología interna con el fin de demostrar que existe la intención de no causar un daño:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Consideración de los indicadores obligatorios de incidencias adversas en materia de sostenibilidad (PIAS) recogidos en el anexo I del Reglamento Delegado (UE) 2022/1288/97, por el que se completa el Reglamento (UE) 2019/2088, tal cual como se describe en la siguiente pregunta.&lt;/li&gt;
+&lt;li&gt;Actividad en sectores controvertidos: mediante el análisis y exclusión de emisores con exposiciones significativas a actividades controvertidas en sectores como combustibles fósiles, armas controvertidas, tabaco, entre otros, así como controversias expuestas a controversias severas.&lt;/li&gt;
+&lt;li&gt;Desempeño sostenible neutro: la Gestora ha requerido una calificación ASG mínima de B en una escala de 7 niveles (C-, C, C+, B, A-, A y A+, donde A+ refleja el mejor desempeño ASG) de acuerdo con su metodología propia para garantizar que las prácticas de sostenibilidad de cada emisor cumplen con unos requisitos ASG mínimos.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Si alguna inversión directa del Fondo ha incumplido con alguna de estas salvaguardas, la Gestora ha considerado que no es posible asegurar que haya existido un daño significativo y no se ha considerado como inversión sostenible&lt;/p&gt;
+&lt;p&gt;En el caso en el que el Plan de Previsión haya invertido en IICs de terceras partes, la Gestora utilizó la metodología de no causar daño significativo divulgada por las gestoras terceras.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Durante el período de referencia, se han adoptado las siguientes medidas para cumplir con las características medioambientales y sociales del Fondo : &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;La Gestora ha revisado periódicamente que el Fondo ha cumplido con las siguientes exclusiones para los activos de inversión directa de contado de emisores, así como los instrumentos financieros derivados (futuros y opciones sobre acciones) utilizados por el Fondo para tomar como referencia el índice en los que el emisor del subyacente de dichos derivados.
+&lt;ul&gt;
+&lt;li&gt;Se han excluido emisores con exposición (medida en términos de volumen de negocios) relacionada con armas controvertidas, y/o con una exposición significativa a combustibles fósiles no convencionales y/o actividades la generación eléctrica a partir del carbón y/o la minería de carbón. &lt;/li&gt;
+&lt;li&gt;Se han excluido del universo de inversiones aquellos emisores en los que se han identificado controversias consideradas críticas en materia medioambiental, social o de gobernanza.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;La Gestora ha supervisado periódicamente que la calificación / rating ASG mínima medio de los emisores de los activos de la cartera de inversión directa de contado, IIC con rating y emisores de los subyacentes de los futuros y opciones sobre acciones utilizados por el Fondo para tomar como referencia el índice, con rating del Fondo ha sido de al menos A-, de acuerdo con la metodología propia de la Gestora en una escala de 7 niveles (C-, C, C+, B, A-, A y A+, donde A+ refleja el mejor desempeño ASG.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Adicionalmente, la Gestora también consideró que los siguientes casos también cumplían con las características medioambientales y sociales promovidas por el Fondo, y se contabilizaban como tal:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Los casos de un emisor sin calificación ASG o que no cumpliera con los indicadores ASG establecidos en la estrategia de inversión, pero que tengan inversiones que puedan ser consideradas inversiones sostenibles, y en concreto emisiones de dicho emisor que puedan ser calificadas como bono verde, social o sostenible, estas emisiones podrían formar parte del universo de activos que promueven las características ASG del Fondo, tras la validación previa de la Gestora, de conformidad con su metodología de análisis propia.&lt;/li&gt;
+&lt;li&gt;Las IICs que, aunque no tengan asignado un rating ASG por la Gestora, sean IICs que promuevan características ASG. (IIC consideradas art. 8 Reglamento (UE) 2019/2088 y/o que tengan como objetivo inversiones sostenibles (art. 9 conforme con el Reglamento (UE) 2019/2088)).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Los criterios ASG anteriores, junto con el cumplimiento de los compromisos mínimos del Fondo se integraron en el proceso de inversión y fueron supervisados periódicamente por el equipo de Cumplimiento de la Gestora. En caso de incumplimiento, se tomaron las medidas correctivas necesarias (por ejemplo, comunicación con el equipo SRI, remisión al comité correspondiente, entre otros).&lt;/p&gt; 
+&lt;p&gt;Además,el desempeño ASG de los emisores ha sido objeto de un seguimiento sistemático y continuo por parte del equipo SRI de la Gestora, incluido el seguimiento continuo de las posibles discrepancias detectadas por los gestores y los datos del modelo proporcionado por los proveedores.&lt;/p&gt;
+&lt;p&gt;Por último, la Gestora ha llevado a cabo actividades de engagement con emisores privados y actividades de voto en los casos en que el tipo de activo lo permite (acciones). Estas actividades estaban alineadas con las características sociales y medioambientales del Fondo y con las Políticas de Engagement y Voto de la Gestora disponibles en https://www.santanderassetmanagement.es/sostenibilidad/. Para ver más ejemplos de las actividades de engagement y voto realizadas, se puede consultar el informe de implicación y voto de la Gestora disponible en: https://www.santanderassetmanagement.es/sostenibilidad/&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Durante el período de referencia, se han adoptado las siguientes medidas para cumplir con las características medioambientales y sociales del Fondo : &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;La Gestora ha revisado periódicamente que el Fondo ha cumplido con las siguientes exclusiones.
+&lt;ul&gt;
+&lt;li&gt;Se han excluido emisores con exposición (medida en términos de volumen de negocios) relacionada con armas controvertidas, y/o con una exposición significativa a combustibles fósiles no convencionales y/o actividades la generación eléctrica a partir del carbón y/o la minería de carbón. &lt;/li&gt;
+&lt;li&gt;Se han excluido del universo de inversiones aquellos emisores en los que se han identificado controversias consideradas críticas en materia medioambiental, social o de gobernanza.&lt;/li&gt;
+&lt;li&gt;Los emisores de renta fija pública fueron evaluados para excluir con aquellos con bajo desempeño en relación con los derechos políticos y libertades sociales. Para ello, la Gestora basó su análisis en cualquiera de los dos indicadores siguientes:&lt;/li&gt;
+&lt;ul&gt;
+&lt;li&gt;Democracy Index: Indicador que determina el rango de democracia de 167 países en base a mediciones tales como el proceso electoral y pluralismo, libertades civiles, funcionamiento del gobierno, participación política y cultura política. En una escala de 1 a 10 puntos, se excluyen los países que  están por debajo de 6 puntos y se corresponden con regímenes híbridos y autoritarios.&lt;/li&gt;
+&lt;li&gt; Estudio Freedom in the World: Indicador que mide el grado de democracia y libertad política en todos los países y en los territorios más importantes en disputa de todo el mundo en una escala de 3 niveles (“No libre”, “Parcialmente libre” y “libre”), se excluyen aquellos países calificados como “No libres”.&lt;/li&gt;&lt;/ul&gt;&lt;/ul&gt;&lt;/li&gt;
+&lt;li&gt;La Gestora ha supervisado periódicamente que la calificación / rating ASG mínima medio de los emisores de los activos de la cartera de inversión directa de contado e IIC con rating del Fondo ha sido de al menos A-, de acuerdo con la metodología propia de la Gestora en una escala de 7 niveles (C-, C, C+, B, A-, A y A+, donde A+ refleja el mejor desempeño ASG).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Adicionalmente, la Gestora también consideró que los siguientes casos también cumplían con las características medioambientales y sociales promovidas por el Fondo, y se contabilizaban como tal:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Los casos de un emisor sin calificación ASG o que no cumpliera con los indicadores ASG establecidos en la estrategia de inversión, pero que tengan inversiones que puedan ser consideradas inversiones sostenibles, y en concreto emisiones de dicho emisor que puedan ser calificadas como bono verde, social o sostenible, estas emisiones podrían formar parte del universo de activos que promueven las características ASG del Fondo, tras la validación previa de la Gestora, de conformidad con su metodología de análisis propia. &lt;/li&gt;
+&lt;li&gt;Las IICs que, aunque no tengan asignado un rating ASG por la Gestora, sean IICs que promuevan características ASG. (IIC consideradas art. 8 Reglamento (UE) 2019/2088 y/o que tengan como objetivo inversiones sostenibles (art. 9 conforme con el Reglamento (UE) 2019/2088)).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Los criter+BX4+BX7</t>
+  </si>
+  <si>
+    <t>¿Cómo se ha comportado este producto financiero en comparación con el índice de referencia designado?</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;¿Cómo se ha comportado este producto financiero con respecto a los indicadores de sostenibilidad para determinar la conformidad del índice de referencia con las características medioambientales o sociales que promueve?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;¿Cómo se ha comportado este producto financiero en comparación con el índice de referencia? &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;¿Cómo se ha comportado este producto financiero en comparación con el índice de referencia designado?&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -1438,12 +1619,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1473,7 +1660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1496,6 +1683,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1834,10 +2027,10 @@
   <dimension ref="A1:CI69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BZ3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1869,7 +2062,7 @@
     <col min="32" max="33" width="26.7265625" customWidth="1"/>
     <col min="34" max="34" width="73.90625" customWidth="1"/>
     <col min="35" max="35" width="26.7265625" customWidth="1"/>
-    <col min="36" max="36" width="73.90625" customWidth="1"/>
+    <col min="36" max="36" width="16.7265625" customWidth="1"/>
     <col min="37" max="38" width="26.7265625" customWidth="1"/>
     <col min="39" max="39" width="73.90625" customWidth="1"/>
     <col min="40" max="41" width="26.7265625" customWidth="1"/>
@@ -2169,7 +2362,7 @@
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2179,7 +2372,7 @@
         <v>59</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>60</v>
@@ -2224,7 +2417,7 @@
         <v>92</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>65</v>
+        <v>217</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>94</v>
@@ -2233,10 +2426,10 @@
         <v>72</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>96</v>
+        <v>222</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>98</v>
@@ -2248,7 +2441,7 @@
         <v>100</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC2" s="3" t="s">
         <v>103</v>
@@ -2332,7 +2525,7 @@
         <v>142</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>141</v>
+        <v>219</v>
       </c>
       <c r="BE2" s="3" t="s">
         <v>140</v>
@@ -2359,13 +2552,13 @@
         <v>158</v>
       </c>
       <c r="BM2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="BN2" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="BN2" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="BO2" s="3" t="s">
-        <v>70</v>
+        <v>221</v>
       </c>
       <c r="BP2" s="3" t="s">
         <v>162</v>
@@ -2374,25 +2567,25 @@
         <v>164</v>
       </c>
       <c r="BR2" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BS2" s="3" t="s">
         <v>166</v>
       </c>
       <c r="BT2" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BU2" s="3" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="BV2" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="BW2" s="3" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="BX2" s="3" t="s">
-        <v>54</v>
+        <v>235</v>
       </c>
       <c r="BY2" s="3" t="s">
         <v>172</v>
@@ -2401,7 +2594,7 @@
         <v>55</v>
       </c>
       <c r="CA2" s="3" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="CB2" s="3" t="s">
         <v>176</v>
@@ -2410,19 +2603,19 @@
         <v>56</v>
       </c>
       <c r="CD2" s="3" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="CE2" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CF2" s="3" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="CG2" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CH2" s="3" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
       <c r="CI2" s="3" t="s">
         <v>56</v>
@@ -2432,7 +2625,7 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2442,7 +2635,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>60</v>
@@ -2505,13 +2698,13 @@
         <v>98</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AA3" s="3" t="s">
         <v>100</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AC3" s="3" t="s">
         <v>103</v>
@@ -2520,7 +2713,7 @@
         <v>104</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AF3" s="3" t="s">
         <v>107</v>
@@ -2553,7 +2746,7 @@
         <v>118</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AQ3" s="3" t="s">
         <v>128</v>
@@ -2592,10 +2785,10 @@
         <v>143</v>
       </c>
       <c r="BC3" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="BD3" s="3" t="s">
-        <v>141</v>
+        <v>219</v>
       </c>
       <c r="BE3" s="3" t="s">
         <v>140</v>
@@ -2604,10 +2797,10 @@
         <v>139</v>
       </c>
       <c r="BG3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="BH3" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="BH3" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="BI3" s="3" t="s">
         <v>155</v>
@@ -2625,13 +2818,13 @@
         <v>51</v>
       </c>
       <c r="BN3" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="BO3" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="BO3" s="3" t="s">
+      <c r="BP3" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="BP3" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="BQ3" s="3" t="s">
         <v>164</v>
@@ -2643,19 +2836,19 @@
         <v>166</v>
       </c>
       <c r="BT3" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BU3" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BV3" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="BV3" s="3" t="s">
+      <c r="BW3" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="BW3" s="3" t="s">
+      <c r="BX3" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="BX3" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="BY3" s="3" t="s">
         <v>172</v>
@@ -2664,7 +2857,7 @@
         <v>55</v>
       </c>
       <c r="CA3" s="3" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="CB3" s="3" t="s">
         <v>176</v>
@@ -2673,30 +2866,30 @@
         <v>56</v>
       </c>
       <c r="CD3" s="3" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="CE3" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CF3" s="3" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="CG3" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CH3" s="3" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
       <c r="CI3" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:87" ht="162" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:87" ht="312.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>211</v>
+      <c r="B4" s="9" t="s">
+        <v>210</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>16</v>
@@ -2705,7 +2898,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>60</v>
@@ -2732,7 +2925,7 @@
         <v>74</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>87</v>
@@ -2747,7 +2940,7 @@
         <v>185</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>186</v>
@@ -2759,7 +2952,7 @@
         <v>187</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>188</v>
@@ -2768,13 +2961,13 @@
         <v>98</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>100</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AC4" s="3" t="s">
         <v>103</v>
@@ -2783,7 +2976,7 @@
         <v>104</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF4" s="3" t="s">
         <v>107</v>
@@ -2816,7 +3009,7 @@
         <v>118</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AQ4" s="3" t="s">
         <v>128</v>
@@ -2855,10 +3048,10 @@
         <v>143</v>
       </c>
       <c r="BC4" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="BD4" s="3" t="s">
-        <v>141</v>
+        <v>219</v>
       </c>
       <c r="BE4" s="3" t="s">
         <v>140</v>
@@ -2867,10 +3060,10 @@
         <v>139</v>
       </c>
       <c r="BG4" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="BH4" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="BH4" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="BI4" s="3" t="s">
         <v>155</v>
@@ -2888,13 +3081,13 @@
         <v>51</v>
       </c>
       <c r="BN4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="BO4" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="BO4" s="3" t="s">
+      <c r="BP4" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="BP4" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="BQ4" s="3" t="s">
         <v>164</v>
@@ -2906,19 +3099,19 @@
         <v>166</v>
       </c>
       <c r="BT4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BU4" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BV4" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="BV4" s="3" t="s">
+      <c r="BW4" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="BW4" s="3" t="s">
+      <c r="BX4" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="BX4" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="BY4" s="3" t="s">
         <v>172</v>
@@ -2927,38 +3120,38 @@
         <v>55</v>
       </c>
       <c r="CA4" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="CB4" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="CB4" s="3" t="s">
-        <v>217</v>
-      </c>
       <c r="CC4" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CD4" s="3" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="CE4" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CF4" s="3" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="CG4" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CH4" s="3" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
       <c r="CI4" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:87" ht="191" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:87" ht="312.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -2968,7 +3161,7 @@
         <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>60</v>
@@ -2995,7 +3188,7 @@
         <v>74</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>87</v>
@@ -3010,10 +3203,10 @@
         <v>185</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="U5" s="3" t="s">
         <v>94</v>
@@ -3022,7 +3215,7 @@
         <v>187</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="X5" s="3" t="s">
         <v>188</v>
@@ -3031,13 +3224,13 @@
         <v>98</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AA5" s="3" t="s">
         <v>100</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AC5" s="3" t="s">
         <v>103</v>
@@ -3046,7 +3239,7 @@
         <v>104</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF5" s="3" t="s">
         <v>107</v>
@@ -3079,7 +3272,7 @@
         <v>118</v>
       </c>
       <c r="AP5" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AQ5" s="3" t="s">
         <v>128</v>
@@ -3118,10 +3311,10 @@
         <v>143</v>
       </c>
       <c r="BC5" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="BD5" s="3" t="s">
-        <v>141</v>
+        <v>219</v>
       </c>
       <c r="BE5" s="3" t="s">
         <v>140</v>
@@ -3130,10 +3323,10 @@
         <v>139</v>
       </c>
       <c r="BG5" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="BH5" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="BH5" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="BI5" s="3" t="s">
         <v>155</v>
@@ -3151,13 +3344,13 @@
         <v>51</v>
       </c>
       <c r="BN5" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BO5" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="BP5" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="BP5" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="BQ5" s="3" t="s">
         <v>164</v>
@@ -3169,19 +3362,19 @@
         <v>166</v>
       </c>
       <c r="BT5" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BU5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BV5" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="BV5" s="3" t="s">
+      <c r="BW5" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="BW5" s="3" t="s">
+      <c r="BX5" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="BX5" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="BY5" s="3" t="s">
         <v>172</v>
@@ -3190,38 +3383,38 @@
         <v>55</v>
       </c>
       <c r="CA5" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="CB5" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="CB5" s="3" t="s">
-        <v>217</v>
-      </c>
       <c r="CC5" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CD5" s="3" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="CE5" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CF5" s="3" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="CG5" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CH5" s="3" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
       <c r="CI5" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:87" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:87" ht="276.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -3231,7 +3424,7 @@
         <v>59</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>76</v>
+        <v>209</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>60</v>
@@ -3246,7 +3439,7 @@
         <v>82</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>83</v>
+        <v>226</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>84</v>
@@ -3267,28 +3460,28 @@
         <v>88</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>90</v>
+        <v>228</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>71</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>92</v>
+        <v>230</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>65</v>
+        <v>217</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>94</v>
+        <v>231</v>
       </c>
       <c r="V6" s="3" t="s">
         <v>72</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>96</v>
+        <v>222</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>45</v>
+        <v>233</v>
       </c>
       <c r="Y6" s="3" t="s">
         <v>98</v>
@@ -3300,7 +3493,7 @@
         <v>100</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="AC6" s="3" t="s">
         <v>103</v>
@@ -3384,7 +3577,7 @@
         <v>142</v>
       </c>
       <c r="BD6" s="3" t="s">
-        <v>141</v>
+        <v>219</v>
       </c>
       <c r="BE6" s="3" t="s">
         <v>140</v>
@@ -3411,13 +3604,13 @@
         <v>158</v>
       </c>
       <c r="BM6" s="3" t="s">
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="BN6" s="3" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="BO6" s="3" t="s">
-        <v>70</v>
+        <v>221</v>
       </c>
       <c r="BP6" s="3" t="s">
         <v>162</v>
@@ -3426,65 +3619,65 @@
         <v>164</v>
       </c>
       <c r="BR6" s="3" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="BS6" s="3" t="s">
         <v>166</v>
       </c>
       <c r="BT6" s="3" t="s">
-        <v>52</v>
+        <v>202</v>
       </c>
       <c r="BU6" s="3" t="s">
         <v>168</v>
       </c>
       <c r="BV6" s="3" t="s">
-        <v>64</v>
+        <v>224</v>
       </c>
       <c r="BW6" s="3" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="BX6" s="3" t="s">
-        <v>54</v>
+        <v>225</v>
       </c>
       <c r="BY6" s="3" t="s">
-        <v>172</v>
+        <v>237</v>
       </c>
       <c r="BZ6" s="3" t="s">
         <v>55</v>
       </c>
       <c r="CA6" s="3" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="CB6" s="3" t="s">
-        <v>176</v>
+        <v>216</v>
       </c>
       <c r="CC6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CD6" s="3" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="CE6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CF6" s="3" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="CG6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CH6" s="3" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
       <c r="CI6" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:87" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:87" ht="276.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -3494,7 +3687,7 @@
         <v>59</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>76</v>
+        <v>209</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>60</v>
@@ -3509,7 +3702,7 @@
         <v>82</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>83</v>
+        <v>226</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>84</v>
@@ -3521,7 +3714,7 @@
         <v>74</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>66</v>
+        <v>227</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>87</v>
@@ -3530,28 +3723,28 @@
         <v>88</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>90</v>
+        <v>228</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>71</v>
+        <v>229</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>92</v>
+        <v>230</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>65</v>
+        <v>217</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>94</v>
+        <v>231</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>72</v>
+        <v>232</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>96</v>
+        <v>222</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>45</v>
+        <v>234</v>
       </c>
       <c r="Y7" s="3" t="s">
         <v>98</v>
@@ -3563,7 +3756,7 @@
         <v>100</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="AC7" s="3" t="s">
         <v>103</v>
@@ -3647,7 +3840,7 @@
         <v>142</v>
       </c>
       <c r="BD7" s="3" t="s">
-        <v>141</v>
+        <v>219</v>
       </c>
       <c r="BE7" s="3" t="s">
         <v>140</v>
@@ -3674,13 +3867,13 @@
         <v>158</v>
       </c>
       <c r="BM7" s="3" t="s">
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="BN7" s="3" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="BO7" s="3" t="s">
-        <v>70</v>
+        <v>221</v>
       </c>
       <c r="BP7" s="3" t="s">
         <v>162</v>
@@ -3689,55 +3882,55 @@
         <v>164</v>
       </c>
       <c r="BR7" s="3" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="BS7" s="3" t="s">
         <v>166</v>
       </c>
       <c r="BT7" s="3" t="s">
-        <v>52</v>
+        <v>202</v>
       </c>
       <c r="BU7" s="3" t="s">
         <v>168</v>
       </c>
       <c r="BV7" s="3" t="s">
-        <v>64</v>
+        <v>224</v>
       </c>
       <c r="BW7" s="3" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="BX7" s="3" t="s">
-        <v>54</v>
+        <v>236</v>
       </c>
       <c r="BY7" s="3" t="s">
-        <v>172</v>
+        <v>237</v>
       </c>
       <c r="BZ7" s="3" t="s">
         <v>55</v>
       </c>
       <c r="CA7" s="3" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="CB7" s="3" t="s">
-        <v>176</v>
+        <v>216</v>
       </c>
       <c r="CC7" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CD7" s="3" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="CE7" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CF7" s="3" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="CG7" s="3" t="s">
         <v>56</v>
       </c>
       <c r="CH7" s="3" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
       <c r="CI7" s="3" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
updated narrative tables with a polish narrative
</commit_message>
<xml_diff>
--- a/excel_books/narratives_tables.xlsx
+++ b/excel_books/narratives_tables.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n740789\Documents\sfdr_report_generator\excel_books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E312057-3F80-4A0D-862D-E33DD2BC5F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46C62F9-CB1C-4C49-9F4E-10BA26425BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{876AE5F7-9A61-4241-A259-03591D994349}"/>
+    <workbookView xWindow="780" yWindow="-16230" windowWidth="14400" windowHeight="16200" activeTab="2" xr2:uid="{876AE5F7-9A61-4241-A259-03591D994349}"/>
   </bookViews>
   <sheets>
-    <sheet name="spanish" sheetId="1" r:id="rId1"/>
-    <sheet name="english" sheetId="2" r:id="rId2"/>
-    <sheet name="polish" sheetId="4" r:id="rId3"/>
-    <sheet name="portuguese" sheetId="3" r:id="rId4"/>
+    <sheet name="es" sheetId="1" r:id="rId1"/>
+    <sheet name="en" sheetId="2" r:id="rId2"/>
+    <sheet name="pl" sheetId="4" r:id="rId3"/>
+    <sheet name="pt" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6052" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6223" uniqueCount="352">
   <si>
     <t>macro_narrative</t>
   </si>
@@ -1866,6 +1866,593 @@
                         La lista incluye las inversiones que constituyen &lt;strong&gt;la mayor parte de las inversiones&lt;/strong&gt;
                         del producto financiero durante el período de referencia, que es: {{ref_period}} 
                     &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Okresowe informacje o produktach finansowych zgodnie z artykułem 8, ustępy 1, 2 i 2 bis rozporządzenia (UE) 2019/2088 oraz artykułem 6, ustęp 1 rozporządzenia (UE) 2020/852</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Identyfikator podmiotu prawnego:&lt;/strong&gt; Kod LEI &lt;span id="lei_code"&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Charakterystyki środowiskowe lub społeczne&lt;/h2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Inwestycja zrównoważona&lt;/strong&gt; oznacza inwestycję w działalność gospodarczą, która przyczynia się do osiągnięcia celu środowiskowego lub społecznego, pod warunkiem że inwestycja nie wyrządza znaczącej szkody żadnemu celowi środowiskowemu lub społecznemu, a przedsiębiorstwa, w które inwestuje, stosują dobre praktyki w zakresie zarządzania.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Taksonomia UE&lt;/strong&gt; to system klasyfikacji przewidziany w rozporządzeniu (UE) 2020/852, który ustanawia listę &lt;strong&gt;działalności gospodarczych środowiskowo zrównoważonych&lt;/strong&gt;. Rozporządzenie to nie zawiera listy działalności gospodarczych społecznie zrównoważonych. Inwestycje zrównoważone mające na celu ochronę środowiska mogą być zgodne lub niezgodne z taksonomią.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- główny kontener pomarańczowego pola --&gt;
+&lt;div class="ob-header"&gt;
+&lt;h2&gt;Czy ten produkt finansowy miał na celu inwestycję zrównoważoną?&lt;/h2&gt;
+&lt;div class="ob-options"&gt;
+&lt;div class="ob-option"&gt;
+&lt;div class="ob-dots"&gt;
+&lt;div class="ob-dot green"&gt;&lt;/div&gt;
+&lt;div class="ob-dot green"&gt;&lt;/div&gt;
+&lt;/div&gt;
+&lt;div class="ob-checkbox"&gt;&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;Tak&lt;/span&gt;
+&lt;/div&gt;
+&lt;div class="ob-option"&gt;
+&lt;div class="ob-dots"&gt;
+&lt;div class="ob-dot green"&gt;&lt;/div&gt;
+&lt;div class="ob-dot white"&gt;&lt;/div&gt;
+&lt;/div&gt;
+&lt;div class="ob-checkbox"&gt;X&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;Nie&lt;/span&gt;
+&lt;/div&gt;
+&lt;/div&gt;
+&lt;/div&gt;
+&lt;div class="ob-body"&gt;
+&lt;div class="ob-columns"&gt;
+&lt;div&gt;
+&lt;div class="ob-item"&gt;
+&lt;div class="ob-checkbox"&gt;&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;&lt;strong&gt;Dokonał inwestycji zrównoważonych w celu środowiskowym:&lt;/strong&gt;&lt;/span&gt;
+&lt;/div&gt;
+&lt;div class="ob-item ob-sub-item"&gt;
+&lt;div class="ob-checkbox"&gt;&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;w działalności gospodarczej uważanej za środowiskowo zrównoważoną zgodnie z taksonomią UE&lt;/span&gt;
+&lt;/div&gt;
+&lt;div class="ob-item ob-sub-item"&gt;
+&lt;div class="ob-checkbox"&gt;&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;w działalności gospodarczej nieuważanej za środowiskowo zrównoważoną zgodnie z taksonomią UE&lt;/span&gt;
+&lt;/div&gt;
+&lt;div class="ob-item"&gt;
+&lt;div class="ob-checkbox"&gt;&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;&lt;strong&gt;Dokonał inwestycji zrównoważonych w celu społecznym:&lt;/strong&gt;&lt;/span&gt;
+&lt;/div&gt;
+&lt;/div&gt;
+&lt;div&gt;
+&lt;div class="ob-item"&gt;
+&lt;div class="ob-checkbox"&gt;X&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;&lt;strong&gt;Promował cechy środowiskowe lub społeczne&lt;/strong&gt;, choć nie miał na celu inwestycji zrównoważonej, osiągnął jednak &lt;span id="sfdr_last_rep_inv_sust_inv"&gt;4,12%&lt;/span&gt; udziału w inwestycjach zrównoważonych&lt;/span&gt;
+&lt;/div&gt;
+&lt;div class="ob-item ob-sub-item"&gt;
+&lt;div class="ob-checkbox"&gt;&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;z celem środowiskowym w działalności gospodarczej uważanej za środowiskowo zrównoważoną zgodnie z taksonomią UE&lt;/span&gt;
+&lt;/div&gt;
+&lt;div class="ob-item ob-sub-item"&gt;
+&lt;div class="ob-checkbox"&gt;X&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;z celem środowiskowym w działalności gospodarczej nieuważanej za środowiskowo zrównoważoną zgodnie z taksonomią UE&lt;/span&gt;
+&lt;/div&gt;
+&lt;div class="ob-item ob-sub-item"&gt;
+&lt;div class="ob-checkbox"&gt;X&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;z celem społecznym&lt;/span&gt;
+&lt;/div&gt;
+&lt;div class="ob-item"&gt;
+&lt;div class="ob-checkbox"&gt;&lt;/div&gt;
+&lt;span class="ob-item-text"&gt;&lt;strong&gt;Promował cechy środowiskowe lub społeczne&lt;/strong&gt;, ale nie dokonał żadnej inwestycji zrównoważonej&lt;/span&gt;
+&lt;/div&gt;
+&lt;/div&gt;
+&lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>W jakim stopniu osiągnięto cechy środowiskowe lub społeczne promowane przez ten produkt finansowy?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Fundusz promował cechy środowiskowe i społeczne, oceniając swoje inwestycje na podstawie kryteriów środowiskowych, społecznych i ładu korporacyjnego (ESG) za pomocą własnej metodologii ESG oraz inwestując w emitentów, którzy wykazują solidne praktyki ESG i spełniają kryteria wykluczenia opisane w strategii inwestycyjnej zawartej w załączniku dotyczącym zrównoważonego rozwoju w informacji przedumownej tego funduszu.
+&lt;/p&gt;
+&lt;p&gt;
+W tym kontekście zastosowano elementy finansowe, środowiskowe, społeczne i dotyczące ładu korporacyjnego, aby uzyskać pełniejszy obraz aktywów bazowych, w które fundusz inwestował w okresie odniesienia, oceniając kombinację czynników ESG, które obejmowały, ale nie ograniczały się do:
+&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Czynniki środowiskowe, poprzez ocenę wyników ilościowych i jakościowych emitentów w zakresie takich zagadnień jak emisje gazów cieplarnianych, wyczerpywanie zasobów, zanieczyszczenia i zarządzanie wodą.
+&lt;/li&gt;
+&lt;li&gt;Czynniki społeczne, obejmujące zagadnienia związane z miejscem pracy, przestrzeganiem standardów pracy, zarządzaniem talentami, relacjami z lokalnymi społecznościami, prywatnością i bezpieczeństwem danych oraz prawami człowieka.
+&lt;/li&gt;
+&lt;li&gt;
+Czynniki dotyczące ładu korporacyjnego, takie jak jakość zarządzania emitenta, jego kultura i etyka, skuteczność systemów ładu korporacyjnego w minimalizowaniu ryzyka niewłaściwego zarządzania oraz zdolność do przewidywania ryzyk operacyjnych i prawnych mogących skutkować naruszeniem. Uwzględniono również czynniki związane ze składem i strukturą rady nadzorczej emitenta.
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;
+Ocena tych czynników dla każdego emitenta opierała się na sektorowej istotności zdefiniowanej przez zarządzającego jako część swojej metodologii ESG. Dodatkowo, przypadki kontrowersji były oceniane, uwzględniając ich wpływ na społeczeństwo, środowisko oraz interesariuszy, i były uwzględniane w metodologii ESG zarządzającego.
+&lt;/p&gt;
+&lt;p&gt;
+Zarządzający promował także cechy środowiskowe i społeczne poprzez działania angażujące, indywidualnie lub w ramach inicjatyw współpracy, mające na celu promowanie lepszych praktyk ESG zgodnie ze swoją polityką zaangażowania.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wskaźniki &lt;strong&gt;zrównoważonego rozwoju&lt;/strong&gt; mierzą, w jakim stopniu osiągane są cechy środowiskowe lub społeczne promowane przez produkt finansowy.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Główne niekorzystne skutki&lt;/strong&gt; to najistotniejsze negatywne skutki decyzji inwestycyjnych dla czynników zrównoważonego rozwoju związanych z kwestiami środowiskowymi, społecznymi, pracowniczymi, przestrzeganiem praw człowieka oraz walką z korupcją i łapownictwem.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;
+                    Jak zachowywały się wskaźniki zrównoważonego rozwoju?
+                &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Poniżej opisano zachowanie wskaźników zrównoważonego rozwoju funduszu w okresie odniesienia:&lt;/p&gt;
+&lt;ul&gt; 
+&lt;li&gt;&lt;strong&gt;Wskaźnik wykluczeń:&lt;/strong&gt; Fundusz nie dokonał żadnych inwestycji w sektory niedozwolone przez politykę inwestycyjną, zgodnie z wewnętrznymi procedurami zarządzającego. To znaczy, że fundusz nie miał ekspozycji na aktywa inwestycyjne bezpośrednio gotówkowe emitentów ani instrumenty pochodne finansowe (futures i opcje na akcje) używane przez fundusz do odniesienia indeksu, w których emitent bazowy tych pochodnych był głównie zaangażowany w działalność związaną z kontrowersyjnym uzbrojeniem, niekonwencjonalnymi paliwami kopalnymi i wytwarzaniem energii elektrycznej z węgla oraz górnictwem węgla.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Wskaźnik kontrowersji:&lt;/strong&gt; Fundusz miał ekspozycję 0% na aktywa inwestycyjne bezpośrednio gotówkowe emitentów, jak również na instrumenty pochodne finansowe (futures i opcje na akcje) używane przez fundusz do odniesienia indeksu, w których emitent bazowy tych pochodnych był zaangażowany w kontrowersje uznawane za krytyczne.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Minimalna średnia ocena ESG funduszu:&lt;/strong&gt; Średnia ocena ESG emitentów aktywów w gotówkowej inwestycyjnej bezpośredniej oraz emitentów bazowych futures i opcji na akcje używanych przez fundusz do odniesienia indeksu według wewnętrznej metodologii zarządzającego wyniosła {{esg_score_2024}} w skali 7 poziomów (C-, C, C+, B, A-, A i A+, gdzie A+ odzwierciedla najlepszy wynik ESG). Wartość tę obliczono jako średnią ocenę ESG, biorąc pod uwagę dane z ostatniego dnia roboczego każdego kwartału w okresie odniesienia.&lt;/li&gt;
+&lt;li&gt;Średni procent aktywów bazowych funduszu zgodnych z cechami środowiskowymi i społecznymi promowanymi wyniósł &lt;strong&gt;{{es_aligned}}%&lt;/strong&gt; w okresie odniesienia.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;
+                    Jak wskaźniki te zachowywały się w porównaniu z wcześniejszymi okresami?
+                &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; W porównaniu z poprzednim okresem odniesienia wyniki wskaźników zrównoważonego rozwoju były następujące:&lt;/p&gt;
+&lt;ul&gt; 
+&lt;li&gt;Wskaźnik wykluczeń: Utrzymał się na poziomie 0%. &lt;/li&gt;
+&lt;li&gt;Wskaźnik kontrowersji: Utrzymał się na poziomie 0%. &lt;/li&gt;
+&lt;li&gt;Minimalna średnia ocena ESG funduszu: W {{YEAR_PREV}} wskaźnik wyniósł {{esg_score_2023}}, a w {{YEAR}} osiągnął {{esg_score_2024}}. &lt;/li&gt;
+&lt;li&gt;Średni procent aktywów bazowych funduszu zgodnych z cechami środowiskowymi i społecznymi promowanymi wyniósł co najmniej 51% w obu okresach odniesienia.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;
+                    Jakie były cele inwestycji zrównoważonych, które częściowo realizował produkt finansowy, i w jaki sposób te inwestycje przyczyniły się do osiągnięcia tych celów?
+                &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Cele inwestycji zrównoważonych tego funduszu osiągnięto poprzez inwestowanie w emitentów, którzy przyczynili się przynajmniej do jednego z celów określonych w Załączniku do Zrównoważonego Rozwoju w informacji przedumownej tego funduszu. W praktyce aktywa bazowe uznane za inwestycje zrównoważone to te emitenci, którzy spełnili przynajmniej jeden z poniższych kryteriów:
+&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+Emitenci, których działalność jest zgodna z trajektorią dekarbonizacji wynikającą z Porozumienia Paryskiego lub jest obecnie neutralna pod względem emisji CO2. Emitenci spełniający to kryterium przyczynili się do osiągnięcia celów środowiskowo zrównoważonych, takich jak łagodzenie zmian klimatycznych, pomagając w stabilizacji koncentracji gazów cieplarnianych w atmosferze i/lub adaptacji do zmian klimatycznych poprzez inwestowanie w rozwiązania adaptacyjne, które znacznie zmniejszają ryzyko negatywnych skutków klimatycznych.
+&lt;/li&gt;
+&lt;li&gt;
+Emitenci, których działalność generuje co najmniej 20% przychodów zgodnych z celami łagodzenia i/lub adaptacji klimatycznej wynikającymi z Taksonomii UE. Na dzień sporządzenia niniejszego dokumentu emitenci spełniający to kryterium przyczynili się do celów środowiskowych związanych z łagodzeniem zmian klimatycznych i/lub adaptacją do tych zmian.
+&lt;/li&gt;
+&lt;li&gt;
+Emitenci generujący co najmniej 20% przychodów z produktów i/lub usług, które mają mierzalny wpływ środowiskowy (np. zrównoważone praktyki rolnicze, technologie zapobiegania zanieczyszczeniom, alternatywne źródła energii). Emitenci spełniający to kryterium przyczynili się do osiągnięcia celów środowiskowo zrównoważonych, takich jak zapobieganie i kontrola zanieczyszczeń, ochrona i odtwarzanie bioróżnorodności oraz ekosystemów, a także zrównoważone wykorzystanie i ochrona zasobów wodnych i morskich.
+&lt;/li&gt;
+&lt;li&gt;
+Emitenci generujący co najmniej 20% przychodów z produktów i/lub usług, które mają mierzalny wpływ społeczny (np. rozwiązania edukacyjne, poprawa łączności, rozwiązania w zakresie leczenia chorób). Emitenci spełniający to kryterium przyczynili się do osiągnięcia celów społecznie zrównoważonych, takich jak zapewnienie odpowiednich standardów życia i dobrostanu konsumentów, przyczyniając się do tworzenia produktów i usług zaspokajających ludzkie potrzeby.
+&lt;/li&gt; 
+&lt;li&gt;
+Emitenci, których praktyki korporacyjne demonstrują ich intencję przyczynienia się do celów środowiskowych i/lub społecznie zrównoważonych funduszu poprzez ich wiodącą ocenę wyników zrównoważoności opartą na metodologii ESG zarządzającego.
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Gdy fundusz inwestował w fundusze inwestycyjne stron trzecich, zarządzający wykorzystywał dane i metodologie zrównoważonych inwestycji ujawnione przez zarządzających stron trzecich.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;W jaki sposób inwestycje zrównoważone, które częściowo realizował produkt finansowy, nie powodowały znaczącej szkody dla żadnego celu zrównoważonego rozwoju środowiskowego lub społecznego?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aby zapewnić, że pozytywny wkład w cel zrównoważonego rozwoju środowiskowego lub społecznego nie spowodował znaczącej szkody dla innych celów zrównoważonych w okresie odniesienia, zarządzający zastosował następujące środki ochrony oparte na swojej wewnętrznej metodologii, aby wykazać, że istnieje zamiar nie wyrządzania takiej szkody:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Uwzględnienie obowiązkowych wskaźników głównych niekorzystnych skutków dla zrównoważonego rozwoju (PIAS) wymienionych w załączniku I rozporządzenia delegowanego (UE) 2022/1288/97, które uzupełnia rozporządzenie (UE) 2019/2088, jak opisano w kolejnym pytaniu.&lt;/li&gt;
+&lt;li&gt;Działalność w kontrowersyjnych sektorach: poprzez analizę i wykluczenie emitentów z istotnym udziałem w działalności kontrowersyjnej w sektorach takich jak paliwa kopalne, broń kontrowersyjna, tytoń oraz emitentów narażonych na poważne kontrowersje.&lt;/li&gt;
+&lt;li&gt;Neutralny wynik zrównoważoności: zarządzający wymagał minimalnej oceny ESG na poziomie B w skali 7 poziomów (C-, C, C+, B, A-, A i A+, gdzie A+ odzwierciedla najlepszy wynik ESG) zgodnie z własną metodologią, aby zagwarantować, że praktyki zrównoważoności każdego emitenta spełniają minimalne wymagania ESG.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;W przypadku gdy jakakolwiek bezpośrednia inwestycja funduszu naruszyła którykolwiek z tych środków ochrony, zarządzający uznał, że nie można zapewnić, że nie doszło do znaczącej szkody i nie została uznana za inwestycję zrównoważoną.&lt;/p&gt;
+&lt;p&gt;Jeżeli program emerytalny inwestował w fundusze inwestycyjne stron trzecich, zarządzający stosował metodologię "nie wyrządzania znaczącej szkody" ujawnioną przez zarządzających stron trzecich.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>W jaki sposób uwzględniono wskaźniki głównych niekorzystnych skutków dla czynników zrównoważonego rozwoju?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Zarządzający uwzględnił obowiązkowe wskaźniki głównych niekorzystnych skutków w analizie zasady "nie wyrządzania znaczącej szkody" dla aktywów bazowych tego funduszu.&lt;/p&gt;
+&lt;p&gt;W tym celu zarządzający zdefiniował progi oparte na kryteriach ilościowych i jakościowych, które obejmowały:&lt;/p&gt;
+&lt;ul&gt;
+    &lt;li&gt;Progi absolutne: emitenci z istotnym udziałem w paliwach kopalnych, działalności wpływającej na obszary wrażliwe biologicznie, naruszający zasady Global Compact ONZ i Wytyczne OECD dla Przedsiębiorstw Wielonarodowych, nieposiadający procesów i mechanizmów monitorowania przestrzegania tych norm międzynarodowych i/lub narażeni na broń kontrowersyjną, zostali uznani za niezgodnych z zasadą "nie wyrządzania znaczącej szkody".&lt;/li&gt;
+    &lt;li&gt;Progi branżowe: emitenci znajdujący się w grupie o najgorszym wyniku w swojej branży pod względem emisji gazów cieplarnianych, emisji do wód, odpadów niebezpiecznych i/lub kwestii społecznych i pracowniczych, zostali uznani za niezgodnych z zasadą "nie wyrządzania znaczącej szkody".&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Czy inwestycje zrównoważone były zgodne z Wytycznymi OECD dla Przedsiębiorstw Wielonarodowych i Zasadami Przewodnimi ONZ dotyczącymi przedsiębiorstw i praw człowieka? Szczegóły:</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Poszanowanie praw człowieka stanowi integralną część wartości zarządzającego oraz minimalny standard działania w celu prowadzenia swojej działalności w sposób zgodny z prawem.&lt;/p&gt;
+&lt;p&gt;W tym kontekście działania zarządzającego opierają się na zasadach określonych w Wytycznych OECD dla Przedsiębiorstw Wielonarodowych oraz dziesięciu zasadach Global Compact ONZ, między innymi. To zaangażowanie odzwierciedla się zarówno w politykach korporacyjnych Grupy Santander, jak i w politykach własnych zarządzającego dostępnych na odpowiednich stronach internetowych i stanowi część wewnętrznego procesu integracji ryzyk zrównoważonego rozwoju zarządzającego.&lt;/p&gt;
+&lt;p&gt;Zarządzający regularnie monitorował, czy bezpośrednie inwestycje gotówkowe naruszają któreś z tych międzynarodowych wytycznych, a w przypadku naruszenia, były one oceniane i zarządzane zgodnie z ich wagą, co mogło prowadzić na przykład do działań zaangażowania.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="obr-content"&gt;
+&lt;p&gt;Taksonomia UE określa zasadę "nie wyrządzania znaczącej szkody", zgodnie z którą inwestycje zgodne z taksonomią nie powinny wyrządzać znaczącej szkody celom taksonomii UE i obejmuje szczególne kryteria unijne.&lt;/p&gt;
+&lt;p&gt;Zasada "nie wyrządzania znaczącej szkody" ma zastosowanie wyłącznie do inwestycji bazowych produktu finansowego, które uwzględniają kryteria UE dotyczące środowiskowo zrównoważonych działań gospodarczych. Inwestycje bazowe pozostałej części produktu finansowego nie uwzględniają tych kryteriów UE.&lt;/p&gt;
+&lt;p class="italic"&gt;Każda inna inwestycja zrównoważona również nie powinna wyrządzać znaczącej szkody żadnemu celowi środowiskowemu lub społecznemu.&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>W jaki sposób ten produkt finansowy uwzględnia główne niekorzystne skutki dla czynników zrównoważonego rozwoju?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Fundusz uwzględnił główne niekorzystne skutki dla czynników zrównoważonego rozwoju podczas podejmowania decyzji inwestycyjnych. Zarządzający stale monitorował wyniki wskaźników z Tabeli 1 oraz dwóch opcjonalnych wskaźników z Tabel 2 i 3 Załącznika I RTS, aby ocenić negatywne skutki, jakie inwestycje realizowane przez ten fundusz mogą powodować w środowisku zewnętrznym.
+&lt;/p&gt;
+&lt;p&gt;
+Podczas okresu odniesienia zarządzający zidentyfikował te skutki na dwóch poziomach:
+&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;
+Na podstawie wyników względnych każdego emitenta, w celu identyfikacji
+emitentów z najgorszymi wynikami w każdym wskaźniku PIAS. Emitenci z najgorszymi wynikami w odniesieniu do swojego sektora dla wszystkich wskaźników obowiązkowych byli oceniani i zarządzani zgodnie z istotnością wpływu i jego powtarzalnością, co mogło prowadzić do działań zaangażowania.
+&lt;/li&gt;
+&lt;li&gt;Na podstawie porównania wskaźników PIAS funduszu z wskaźnikami indeksu odniesienia (benchmark). Kiedy wyniki funduszu były gorsze niż wyniki benchmarku, zarządzający analizował wagę wpływu, jego powtarzalność w czasie, prawdopodobieństwo sukcesu działań zaangażowania, ekspozycję portfela oraz rodzaj wskaźnika PIAS, aby wdrożyć działania łagodzące. Podczas okresu odniesienia działania te były priorytetowe dla wskaźników związanych z emisjami gazów cieplarnianych i/lub naruszeniami Global Compact ONZ. Zarządzający łagodził również te negatywne skutki, dostosowując pozycje najbardziej przyczyniające się do najgorszych wyników PIAS w porównaniu z benchmarkiem, ograniczając zwiększenie pozycji lub w ostateczności poprzez dezinwestycję.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;
+Dane potrzebne do obliczenia wskaźników PIAS były dostarczane przez zewnętrznych dostawców danych. Przeprowadzano regularną analizę jakości i pokrycia danych we współpracy z emitentami i dostawcami danych, aby rozwiązać ograniczenia w dostępności i jakości danych wskaźników.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Jakie były główne inwestycje tego produktu finansowego?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lista zawiera inwestycje, które stanowiły &lt;strong&gt;większość inwestycji&lt;/strong&gt; produktu finansowego w okresie odniesienia, tj.: {{ref_period}}&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Główne inwestycje Programu Emerytalnego dokonane w okresie odniesienia to:&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;table&gt;
+&lt;colgroup&gt;
+&lt;col class="col1"/&gt;
+&lt;col class="col2"/&gt;
+&lt;col class="col3"/&gt;
+&lt;col class="col4"/&gt;
+&lt;/colgroup&gt;
+&lt;thead&gt;
+&lt;tr&gt;
+&lt;th&gt;Najważniejsze inwestycje&lt;/th&gt;
+&lt;th&gt;Sektor&lt;/th&gt;
+&lt;th style="text-align: center;"&gt;% aktywów&lt;/th&gt;
+&lt;th style="text-align: center;"&gt;Kraj&lt;/th&gt;
+&lt;/tr&gt;
+&lt;/thead&gt;
+&lt;tbody&gt;
+&lt;tr&gt;
+&lt;td&gt;SPAIN (KINGDOM OF) 0 31/01/27 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;11,61%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;BONOS Y OBLIG DEL EST 0.8 30/07/25 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;10,61%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;BONOS Y OBLIG DEL ESTADO 0 31/01/26 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;10,28%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;SPAIN (KINGDOM OF) 2.8 31/05/26 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;8,29%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;SPAIN (KINGDOM OF) 0 31/05/25 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;7,77%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;BONOS Y OBLIG DEL ESTADO 1.25 31/10/30&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;5,02%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;BONOS Y OBLIG DEL EST 0.7 30/04/32 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;5,01%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;BONOS Y OBLIG DEL EST 2.55 10/32 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;4,12%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;BONOS Y OBLIG DEL ESTADO 0.5 30/04/30 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;3,45%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;SPAIN (KINGDOM OF) 3.55 31/10/33 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;3,17%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;/tbody&gt;
+&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t>&lt;table&gt;
+&lt;colgroup&gt;
+&lt;col class="col1"/&gt;
+&lt;col class="col2"/&gt;
+&lt;col class="col3"/&gt;
+&lt;col class="col4"/&gt;
+&lt;/colgroup&gt;
+&lt;thead&gt;
+&lt;tr&gt;
+&lt;th&gt;Najważniejsze inwestycje&lt;/th&gt;
+&lt;th&gt;Sektor&lt;/th&gt;
+&lt;th style="text-align: center;"&gt;% aktywów&lt;/th&gt;
+&lt;th style="text-align: center;"&gt;Kraj&lt;/th&gt;
+&lt;/tr&gt;
+&lt;/thead&gt;
+&lt;tbody&gt;
+&lt;tr&gt;
+&lt;td&gt;FRANCE (REPUBLIC OF) 0 25/05/26 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;2,95%&lt;/td&gt;
+&lt;td class="country"&gt;FR&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;FRANCE (REPUBLIC OF) 1 25/05/27 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;2,71%&lt;/td&gt;
+&lt;td class="country"&gt;FR&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;BONOS Y OBLIG DEL ESTADO 3.8 30/07/42 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;2,44%&lt;/td&gt;
+&lt;td class="country"&gt;ES&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;FRANCE (REPUBLIC OF) 2.75 25/10/27 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;2,29%&lt;/td&gt;
+&lt;td class="country"&gt;FR&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;ITALY (REPUBLIC OF) 0.95 01/03/23 (EUR)&lt;/td&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent"&gt;1,78%&lt;/td&gt;
+&lt;td class="country"&gt;IT&lt;/td&gt;
+&lt;/tr&gt;
+&lt;/tbody&gt;
+&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t>W jakich sektorach gospodarczych dokonano inwestycji?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sektory gospodarcze, w które zainwestowano w okresie odniesienia, to:&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Procent inwestycji zrównoważonych został obliczony jako udział aktywów bazowych spełniających kryteria zrównoważoności w stosunku do całkowitego majątku funduszu. Zostały wzięte pod uwagę aktywa z cechami środowiskowymi lub społecznymi, które spełniały wymagania określone w taksonomii UE.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Jakie są sektory gospodarcze, w które inwestowano?</t>
+  </si>
+  <si>
+    <t>Sektory gospodarcze, w które inwestowano w okresie odniesienia, to przedstawione poniżej.</t>
+  </si>
+  <si>
+    <t>&lt;div class="obr-content"&gt;Opis sektorów gospodarczych i ich wpływu na inwestycje.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;svg class="flowchart-lines"&gt;&lt;/svg&gt;
+&lt;div class="nodes"&gt;
+&lt;div class="node" id="n10000"&gt;Inwestycje&lt;/div&gt;
+&lt;div class="branch-horizontal"&gt;
+&lt;div class="node" id="n11000" data-parent="n10000"&gt;n.º 1 Dostosowane do cech środowiskowych lub społecznych&lt;/div&gt;
+&lt;div class="node" id="n12000" data-parent="n10000"&gt;n.º 2 Pozostałe&lt;/div&gt;
+&lt;/div&gt;
+&lt;div class="branch-horizontal"&gt;
+&lt;div class="node" id="n11100" data-parent="n11000"&gt;n.º 1A Zrównoważone&lt;/div&gt;
+&lt;div class="node" id="n11200" data-parent="n11000"&gt;n.º 1B Pozostałe cechy środowiskowe lub społeczne&lt;/div&gt;
+&lt;/div&gt;
+&lt;div class="sub-branch-horizontal"&gt;
+&lt;div class="node" id="n11110" data-parent="n11100"&gt;Inne środowiskowe&lt;/div&gt;
+&lt;div class="node" id="n11120" data-parent="n11100"&gt;Społeczne&lt;/div&gt;
+&lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Inwestycje</t>
+  </si>
+  <si>
+    <t>n.º 1 Dostosowane do cech środowiskowych lub społecznych</t>
+  </si>
+  <si>
+    <t>n.º 2 Pozostałe</t>
+  </si>
+  <si>
+    <t>n.º 1A Zrównoważone</t>
+  </si>
+  <si>
+    <t>n.º 1B Pozostałe cechy środowiskowe lub społeczne</t>
+  </si>
+  <si>
+    <t>Inne środowiskowe</t>
+  </si>
+  <si>
+    <t>Społeczne</t>
+  </si>
+  <si>
+    <t>Jakie sektory gospodarcze były zaangażowane?</t>
+  </si>
+  <si>
+    <t>Sektory gospodarcze zaangażowane w inwestycje to następujące:</t>
+  </si>
+  <si>
+    <t>&lt;table&gt;
+&lt;colgroup&gt;
+&lt;col class="col1"/&gt;
+&lt;col class="col2"/&gt;
+&lt;/colgroup&gt;
+&lt;thead&gt;
+&lt;tr&gt;
+&lt;th&gt;Sektor gospodarczy&lt;/th&gt;
+&lt;th style="text-align: center;"&gt;Alokacja aktywów w %&lt;/th&gt;
+&lt;/tr&gt;
+&lt;/thead&gt;
+&lt;tbody&gt;
+&lt;tr&gt;
+&lt;td&gt;Administracja publiczna i obrona; Obowiązkowe ubezpieczenia społeczne&lt;/td&gt;
+&lt;td class="percent" style="text-align: center;"&gt;94,24%&lt;/td&gt;
+&lt;/tr&gt;
+&lt;tr&gt;
+&lt;td&gt;Działalność finansowa i ubezpieczeniowa&lt;/td&gt;
+&lt;td class="percent" style="text-align: center;"&gt;5,76%&lt;/td&gt;
+&lt;/tr&gt;
+&lt;/tbody&gt;
+&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t>W jakim stopniu zrównoważone inwestycje mające cel środowiskowy były zgodne z taksonomią UE?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Działania wspierające&lt;/strong&gt; bezpośrednio umożliwiają innym działaniom znaczące przyczynienie się do osiągnięcia celu środowiskowego.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Działania przejściowe&lt;/strong&gt; to działania, dla których nie istnieją jeszcze alternatywy o niskiej emisji dwutlenku węgla i które charakteryzują się poziomami emisji gazów cieplarnianych zgodnymi z najlepszymi wynikami w branży.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aktywności zgodne z taksonomią UE są przedstawione jako procent:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;&lt;strong&gt;Obrotu:&lt;/strong&gt; który odzwierciedla procent przychodów uzyskanych z działalności ekologicznej przedsiębiorstw, w które inwestuje fundusz.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Inwestycji w aktywa trwałe (CapEx):&lt;/strong&gt; które pokazują inwestycje ekologiczne realizowane przez przedsiębiorstwa, w które inwestuje fundusz, np. przejście na zieloną gospodarkę.&lt;/li&gt;
+&lt;li&gt;&lt;strong&gt;Kosztów operacyjnych (OpEx):&lt;/strong&gt; które odzwierciedlają działalność operacyjną przedsiębiorstw, w które inwestuje fundusz, zgodną z celem środowiskowym.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Fundusz nie określił minimalnego procentu zgodności swoich inwestycji z taksonomią UE ani nie miał celu inwestycyjnego zgodnego z nią. W związku z tym dane te nie podlegają audytowi i są przedstawiane wyłącznie w celach informacyjnych. Poniższe wykresy przedstawiają zgodność funduszu z taksonomią UE w okresie odniesienia. Dane są przedstawiane wyłącznie informacyjnie, ponieważ nie odzwierciedlają zgodności z żadnym celem ani minimalnym zobowiązaniem inwestycyjnym.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;Czy produkt finansowy inwestował w działania związane z gazem kopalnym lub energią jądrową, które spełniały taksonomię UE&lt;sup&gt;1&lt;/sup&gt;?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;label&gt;
+&lt;input type="checkbox"/&gt;
+&lt;span&gt;Nie&lt;/span&gt;
+&lt;/label&gt;</t>
+  </si>
+  <si>
+    <t>&lt;hr/&gt;
+&lt;p&gt;&lt;sup&gt;1&lt;/sup&gt;Działania związane z gazem kopalnym lub energią jądrową spełniają taksonomię UE tylko wtedy, gdy przyczyniają się do ograniczenia zmian klimatycznych ("łagodzenie zmian klimatycznych") i nie wyrządzają znaczącej szkody żadnemu celowi taksonomii UE. Pełne kryteria dotyczące działań gospodarczych związanych z gazem kopalnym i energią jądrową zgodnych z taksonomią UE określono w rozporządzeniu delegowanym Komisji (UE) 2022/1214.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;Jaki był udział inwestycji w działania przejściowe i wspierające?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Udział inwestycji w działania przejściowe wyniósł {{total_turnover_transition}} w obrotach, {{total_capex_transition}} w nakładach inwestycyjnych (CapEx) i {{total_opex_transition}} w kosztach operacyjnych (OpEx), a w działania wspierające {{total_turnover_enabling}} w obrotach, {{total_capex_enabling}} w CapEx i {{total_opex_enabling}} w OpEx w odniesieniu do całkowitego majątku funduszu w okresie odniesienia.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;Jaki procent inwestycji był zgodny z taksonomią UE w porównaniu z wcześniejszymi okresami odniesienia?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Fundusz nie określił minimalnego procentu zgodności swoich inwestycji z taksonomią UE. Niemniej jednak, zgodność inwestycji z taksonomią UE w porównaniu z okresem odniesienia wyniosła {{taxonomy_2022}}, {{taxonomy_2023}}, a w {{taxonomy_2024}} osiągnęła {{total_turnover_aligned}}.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Jaki był udział inwestycji zrównoważonych z celem środowiskowym, które nie były zgodne z taksonomią UE?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Inwestycje zrównoważone z celem środowiskowym&lt;/strong&gt; to inwestycje, które &lt;strong&gt;nie uwzględniają kryteriów&lt;/strong&gt; środowiskowej zgodności działań gospodarczych z taksonomią UE, zgodnie z rozporządzeniem (UE) 2020/852.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Udział inwestycji zrównoważonych funduszu z celem środowiskowym, które nie były zgodne z taksonomią UE, wyniósł {{sust_invest_env}}% w okresie odniesienia.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Jaki był udział inwestycji społecznie zrównoważonych?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Udział inwestycji społecznie zrównoważonych funduszu wyniósł {{sust_invest_soc}}% w okresie odniesienia.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Jakie inwestycje zostały uwzględnione w kategorii "inne" i jaki był ich cel? Czy były stosowane minimalne zabezpieczenia środowiskowe lub społeczne?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Fundusz uwzględnił {{other_nones}}% majątku funduszu w okresie odniesienia w inwestycjach, które nie są zgodne z cechami środowiskowymi i społecznymi promowanymi przez fundusz. Odsetek ten obliczono jako średni udział majątku funduszu, uwzględniając inwestycje bazowe z ostatniego dnia roboczego każdego kwartału okresu odniesienia, zgodnie z definicją w sekcji "Główne inwestycje".&lt;/p&gt;
+&lt;p&gt;Inwestycje te nie wpłynęły negatywnie na osiągnięcie cech środowiskowych i społecznych promowanych przez fundusz, a ich celem było wspieranie efektywnego zarządzania portfelem, zapewnianie płynności oraz funkcja zabezpieczająca.&lt;/p&gt;
+&lt;p&gt;Minimalne zabezpieczenia środowiskowe i społeczne obejmowały:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Bezpośrednie aktywa inwestycyjne bez ratingu ESG z powodu braku danych dostawcy wykorzystywanego przez zarządzającego, które nie mogą być uznane za inwestycje zrównoważone. Te aktywa spełniały kryteria wykluczeń funduszu, zapewniając minimalne zabezpieczenia.&lt;/li&gt;
+&lt;li&gt;Fundusze inwestycyjne bez ratingu ESG z powodu braku danych, które nie mogą być klasyfikowane jako fundusze zgodne z art. 8 lub 9 Rozporządzenia (UE) 2019/2088. W procesie selekcji funduszy stosowano minimalne zabezpieczenia zgodne z procedurami zarządzającego.&lt;/li&gt;
+&lt;li&gt;Inne aktywa gotówkowe dopuszczalne zgodnie z polityką funduszu, dla których stosowano minimalne zabezpieczenia.&lt;/li&gt;
+&lt;li&gt;Płynność w depozytariuszu i inne rachunki bieżące wykorzystywane do zwykłej działalności funduszu (np. zabezpieczenia instrumentów pochodnych).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;W przypadku instrumentów finansowych pochodnych (oprócz kontraktów terminowych i opcji na akcje wykorzystywanych do odniesienia indeksu), nie stosowano powyższych procedur w zakresie promocji cech ESG, z wyjątkiem określonych sytuacji.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Jakie działania podjęto, aby spełnić cechy środowiskowe lub społeczne w okresie odniesienia?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;W okresie odniesienia podjęto następujące działania, aby spełnić cechy środowiskowe i społeczne funduszu:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Zarządzający regularnie weryfikował, czy fundusz przestrzega następujących kryteriów wykluczenia dla aktywów inwestycyjnych:
+&lt;ul&gt;
+&lt;li&gt;Wykluczono emitentów z ekspozycją na sektory takie jak broń kontrowersyjna, paliwa kopalne niekonwencjonalne, wytwarzanie energii z węgla oraz górnictwo węglowe.&lt;/li&gt;
+&lt;li&gt;Wykluczono emitentów, w których zidentyfikowano kontrowersje uznane za krytyczne w zakresie środowiskowym, społecznym lub zarządzania.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Zarządzający regularnie monitorował minimalny średni rating ESG aktywów inwestycyjnych funduszu, który wynosił co najmniej A-, zgodnie z metodologią zarządzającego na siedmiostopniowej skali (C-, C, C+, B, A-, A, A+).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Dodatkowo, zarządzający uznawał za zgodne z cechami środowiskowymi i społecznymi funduszu następujące przypadki:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Emitenci bez ratingu ESG, ale posiadający inwestycje, które mogą być uznane za zrównoważone, takie jak zielone obligacje.&lt;/li&gt;
+&lt;li&gt;Fundusze inwestycyjne promujące cechy środowiskowe lub społeczne zgodnie z art. 8 lub 9 Rozporządzenia (UE) 2019/2088.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Wszystkie powyższe kryteria były integrowane w procesie inwestycyjnym i monitorowane przez zespół ds. zgodności zarządzającego. W przypadku naruszenia podejmowano działania naprawcze, takie jak komunikacja z zespołem SRI czy skierowanie sprawy do odpowiedniego komitetu.&lt;/p&gt;
+&lt;p&gt;Zarządzający prowadził również działania angażujące z emitentami oraz głosowania na walnych zgromadzeniach, aby wspierać cele środowiskowe i społeczne funduszu.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Jak produkt finansowy zachowywał się w porównaniu z wyznaczonym indeksem odniesienia?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nie wyznaczono konkretnego indeksu jako punktu odniesienia do określenia, czy ten produkt finansowy spełnia promowane cechy środowiskowe lub społeczne.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Indeksy odniesienia&lt;/strong&gt; to wskaźniki stosowane do pomiaru, czy produkt finansowy osiąga promowane cechy środowiskowe lub społeczne.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;W jaki sposób indeks odniesienia różni się od ogólnego indeksu rynkowego?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nie dotyczy.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;Jak produkt finansowy zachowywał się w odniesieniu do wskaźników zrównoważoności w celu określenia zgodności indeksu odniesienia z promowanymi cechami środowiskowymi lub społecznymi?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sub-qtext"&gt;Jak produkt finansowy zachowywał się w porównaniu z wyznaczonym indeksem odniesienia?&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="obr-content"&gt;
+&lt;p&gt;&lt;i&gt;Wykresy poniżej przedstawiają w zielonym kolorze procent inwestycji zgodnych z taksonomią UE. Ze względu na brak odpowiedniej metodologii do określania zgodności obligacji skarbowych z taksonomią, pierwszy wykres przedstawia zgodność z taksonomią dla wszystkich inwestycji funduszu, w tym obligacji skarbowych, podczas gdy drugi wykres pokazuje zgodność z taksonomią wyłącznie dla inwestycji innych niż obligacje skarbowe.&lt;/i&gt;&lt;/p&gt;
+&lt;!--Add graph image--&gt;
+&lt;div class="chart"&gt;
+&lt;img 
+src="graphs_plots\plot_orb_full.png"
+alt="Ajuste a la taxonomía de las inversiones." /&gt;
+&lt;/div&gt;
+&lt;p style="font-style: italic"&gt;*Na potrzeby tych wykresów "obligacje skarbowe" obejmują wszystkie ekspozycje skarbowe.&lt;/i&gt;&lt;/p&gt;
+&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -2336,11 +2923,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2CF707-1372-4610-A1C4-0399A26E6B10}">
   <dimension ref="A1:CG69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="BE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="BE16" sqref="BE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19827,6 +20414,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -20205,12 +20793,537 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6A6837-7230-4429-B7FC-980D5EFB5D43}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:CH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="BI2" sqref="BI2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="60" width="21" customWidth="1"/>
+    <col min="61" max="61" width="74.7265625" customWidth="1"/>
+    <col min="62" max="86" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:86" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="BT1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="BU1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BV1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="BW1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BX1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BY1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BZ1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CA1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CB1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CC1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CD1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="CE1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="CF1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="CH1" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:86" s="3" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="BG2" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="BH2" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="BK2" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="BL2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="BM2" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="BN2" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="BO2" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="BP2" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="BQ2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="BR2" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="BS2" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="BT2" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="BU2" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="BV2" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="BW2" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="BX2" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="BZ2" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="CA2" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="CB2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="CC2" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="CD2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="CE2" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="CF2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="CG2" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="CH2" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20220,7 +21333,7 @@
   <dimension ref="A1:CI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20757,6 +21870,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee51a08e-cffb-442e-9a85-1980beacc2f8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9f04ef3f-090d-46e3-96be-1fbea4829461" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EA6A4DE027E6E4386DF60BFAE3B87E5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17b8f265623aebada2f4fbb4af048074">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee51a08e-cffb-442e-9a85-1980beacc2f8" xmlns:ns3="9f04ef3f-090d-46e3-96be-1fbea4829461" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="76d895b679038352f9e7e02d8518f5a2" ns2:_="" ns3:_="">
     <xsd:import namespace="ee51a08e-cffb-442e-9a85-1980beacc2f8"/>
@@ -20963,41 +22096,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee51a08e-cffb-442e-9a85-1980beacc2f8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9f04ef3f-090d-46e3-96be-1fbea4829461" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9D26033-77B4-4FF0-A22A-B37DD9FF0884}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF03F5EE-765F-4A4C-B279-DCB1DCEB979E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ee51a08e-cffb-442e-9a85-1980beacc2f8"/>
-    <ds:schemaRef ds:uri="9f04ef3f-090d-46e3-96be-1fbea4829461"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -21020,9 +22122,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF03F5EE-765F-4A4C-B279-DCB1DCEB979E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9D26033-77B4-4FF0-A22A-B37DD9FF0884}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee51a08e-cffb-442e-9a85-1980beacc2f8"/>
+    <ds:schemaRef ds:uri="9f04ef3f-090d-46e3-96be-1fbea4829461"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated narrative tables excel
</commit_message>
<xml_diff>
--- a/excel_books/narratives_tables.xlsx
+++ b/excel_books/narratives_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n740789\Documents\sfdr_report_generator\excel_books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E13BA6-857B-4EBC-8758-4F83602FABC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A139D95-3A97-41FC-93D6-9241852F9990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13740" yWindow="-16350" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{876AE5F7-9A61-4241-A259-03591D994349}"/>
+    <workbookView xWindow="15360" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{876AE5F7-9A61-4241-A259-03591D994349}"/>
   </bookViews>
   <sheets>
     <sheet name="es" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="561">
   <si>
     <t>macro_narrative</t>
   </si>
@@ -2185,9 +2185,6 @@
     <t>What was the share of investments made in transitional and enabling activities?</t>
   </si>
   <si>
-    <t>The proportion of investments made in transition activities has been {{total_turnover_enabling}} in turnover, in {{total_capex_enabling}} CapEx and in {{total_opex_enabling}} OpEx and in activities facilitating {{total_turnover}} in turnover}, {{total_capex_transition}} in CapEx and {{TOTAL_opex_TRANSION}} in OpEx over the reference period.</t>
-  </si>
-  <si>
     <t>How did the percentage of investments that were aligned with the EU Taxonomy compare with previous reference periods?</t>
   </si>
   <si>
@@ -2213,9 +2210,6 @@
   </si>
   <si>
     <t>How did this financial product perform compared to the reference benchmark?</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>&lt;b&gt;Reference benchmarks &lt;/b&gt; are indexes to measure whether the financial product attains the environmental or social characteristics that they promote.</t>
@@ -2313,9 +2307,6 @@
   </si>
   <si>
     <t>em atividades económicas que não são qualificadas como sustentáveis do ponto de vista ambiental ao abrigo da taxonomia da UE</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Promoveu características ambientais/ sociais (A/S)&lt;/b&gt;e, apesar de não ter como objetivo a realização de um investimento sustentável, consagrou uma percentagem mínima de &lt;span id="sfdr_last_rep_inv_sust_inv"&gt;&lt;/span&gt;% a investimentos sustentáveis</t>
   </si>
   <si>
     <t>com um objetivo ambiental em atividades económicas qualificadas como sustentáveis do ponto de vista ambiental ao abrigo da taxonomia da UE</t>
@@ -2700,19 +2691,6 @@
     <t xml:space="preserve"> The Sub-Fund does not have a minimum percentage of alignment of its investments with the EU Taxonomy. However, the percentage of investments aligned with the EU Taxonomy compared to the previous reference periods has been  {{taxonomy_2022}} {{taxonomy_2023}} and {{total_turnover_aligned}} in 2024.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;The financial product had a  {{other_nones}}% share of investments which are neither aligned with the environmental or social characteristics, nor are qualified as sustainable investments. This percentage was calculated as the average percentage of the Sub-Fund considering the underlying investments from the last business day of each quarter of the reference period as defined in the Top Investments section.&lt;/p&gt;
-&lt;p style="margin-top: -10px;"&gt;                   
-These investments did not alter the achievement of the environmental or social characteristics promoted by the Sub-Fund, and their purpose was investment, contributing to efficient portfolio management, providing liquidity and hedging.&lt;/p&gt;
-&lt;p style="margin-top: -10px;"&gt; The Investment Manager has established minimum environmental or social safeguards so as not to cause significant damage, such as consideration of the principal adverse impacts, or the exclusion of activities that are not aligned with the environmental and/or social characteristics of the Fund. The assets that could be considered were the following:&lt;/p&gt;
-&lt;ul&gt;
-                    &lt;li&gt;Direct cash investment assets that did not have an ESG rating/rating due to the lack of supplier data used by the Investment Manager and which cannot be considered sustainable investments in accordance with the criterion defined in the previous section (i.e., green, social bonds, etc.).&lt;/li&gt;
-                    &lt;li&gt;Investment funds that did not have an ESG rating/rating due to lack of data and that cannot be classified as an investment Sub-Fund art. 8 or 9 according to SFDR.&lt;/li&gt;
-                    &lt;li&gt;Other cash assets other than those mentioned above. (i.e., ETC, etc.) that are permitted by the Sub-Fund's policy and do not harm its ESG profile.&lt;/li&gt;
-                    &lt;li&gt;Other cash assets other than those mentioned above. (i.e., ETC, etc.) that are permitted by the Sub-Fund's policy and do not harm its ESG profile.&lt;/li&gt;
-&lt;/ul&gt;
-</t>
-  </si>
-  <si>
     <t>&lt;p&gt;
   During the reference period, the following actions have been taken
   to meet the environmental and social characteristics of the
@@ -3147,9 +3125,6 @@
 </t>
   </si>
   <si>
-    <t>&lt;p&gt;N/A&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;The Sub-Fund has promoted environmental and social characteristics by evaluating its underlying investments against environmental, social, and governance (ESG) criteria using a proprietary ESG methodology and investing in issuers that exhibit sound ESG practices and comply with the exclusion factors described in the Sub-Fund’s investment strategy.&lt;/p&gt;
 &lt;p&gt;In this sense, financial, environmental, social, and good governance elements have been used to obtain a more complete view of the assets in which the Sub-Fund invested during the reference period, having evaluated a combination of ESG factors that included but were not limited to:&lt;/p&gt;
 &lt;ul&gt;
@@ -3418,15 +3393,6 @@
     <t>Promoveu características (A/S), mas &lt;b&gt;não realizou quaisquer investimento sustentáveis&lt;/b&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt; O desempenho dos indicadores de sustentabilidade do Fundo ao longo do período de referência é abaixo descrito&lt;/p&gt;
-&lt;ul&gt; 
-&lt;li&gt; Indicador de exclusões: o Fundo não realizou qualquer investimento em setores não permitidos pela respetiva política de investimento. Ou seja, o Fundo excluiu, entre outros, emitentes cujo negócio esteja principalmente orientado para atividades relacionadas com armamento controverso e convencional, tabaco, bem como combustíveis fósseis, produção de eletricidade a partir de carvão e extração de carvão. Adicionalmente, no caso das obrigações governamentais, o Fundo teve 0% de exposição a países com fraco desempenho em termos de direitos políticos e liberdades sociais, considerando o indicador Democracy Index e o estudo Freedom in the World.. &lt;/li&gt;
-&lt;li&gt;Indicador de controvérsias: o Fundo teve 0% de exposição a empresas que estiveram envolvidas em controvérsias consideradas críticas.&lt;/li&gt;
-&lt;li&gt;Classificação (rating) média ASG do Fundo: a classificação ASG média dos ativos que compõem a carteira de investimento do Fundo, classificados de acordo com a metodologia interna da Sociedade Gestora, foi de {{esg_score_2024}} numa escala de 7 níveis (C-, C, C+, B, A-, A e A+, em que A+ reflete o melhor desempenho ASG). Este valor foi calculado como a média de rating ASG dos produtos/ativos que compõem a carteira com rating ASG, considerando os dados do último dia útil de cada trimestre do período de referência, tal como definido na secção Principais Investimentos.&lt;/li&gt;
-&lt;li&gt;Percentagem de ativos do Fundo alinhados com as características ambientais e sociais promovidas foi de {{es_aligned}}.&lt;/li&gt;
-&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>...e em relação a períodos anteriores?</t>
   </si>
   <si>
@@ -3460,6 +3426,36 @@
   </si>
   <si>
     <t>Realizou &lt;b&gt;investimentos sustentáveis com um objetivo social:&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Promoveu características ambientais/ sociais (A/S)&lt;/b&gt; e, apesar de não ter como objetivo a realização de um investimento sustentável, consagrou uma percentagem mínima de &lt;span id="sfdr_last_rep_inv_sust_inv"&gt;&lt;/span&gt;% a investimentos sustentáveis</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; O desempenho dos indicadores de sustentabilidade do Fundo ao longo do período de referência é abaixo descrito&lt;/p&gt;
+&lt;ul&gt; 
+&lt;li&gt; Indicador de exclusões: o Fundo não realizou qualquer investimento em setores não permitidos pela respetiva política de investimento. Ou seja, o Fundo excluiu, entre outros, emitentes cujo negócio esteja principalmente orientado para atividades relacionadas com armamento controverso e convencional, tabaco, bem como combustíveis fósseis, produção de eletricidade a partir de carvão e extração de carvão. Adicionalmente, no caso das obrigações governamentais, o Fundo teve 0% de exposição a países com fraco desempenho em termos de direitos políticos e liberdades sociais, considerando o indicador Democracy Index e o estudo Freedom in the World.. &lt;/li&gt;
+&lt;li&gt;Indicador de controvérsias: o Fundo teve 0% de exposição a empresas que estiveram envolvidas em controvérsias consideradas críticas.&lt;/li&gt;
+&lt;li&gt;Classificação (rating) média ASG do Fundo: a classificação ASG média dos ativos que compõem a carteira de investimento do Fundo, classificados de acordo com a metodologia interna da Sociedade Gestora, foi de {{esg_score_2024}} numa escala de 7 níveis (C-, C, C+, B, A-, A e A+, em que A+ reflete o melhor desempenho ASG). Este valor foi calculado como a média de rating ASG dos produtos/ativos que compõem a carteira com rating ASG, considerando os dados do último dia útil de cada trimestre do período de referência, tal como definido na secção Principais Investimentos.&lt;/li&gt;
+&lt;li&gt;Percentagem de ativos do Fundo alinhados com as características ambientais e sociais promovidas foi de {{es_aligned}}%.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>The proportion of investments made in transition activities has been {{total_turnover_enabling}} in turnover, in {{total_capex_enabling}} CapEx and in {{total_opex_enabling}} OpEx and in activities facilitating {{total_turnover}} in turnover, {{total_capex_transition}} in CapEx and {{total_opex_transition}} in OpEx over the reference period.</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;The financial product had a  {{other_nones}}% share of investments which are neither aligned with the environmental or social characteristics, nor are qualified as sustainable investments. This percentage was calculated as the average percentage of the Sub-Fund considering the underlying investments from the last business day of each quarter of the reference period as defined in the Top Investments section.&lt;/p&gt;
+&lt;p style="margin-top: -10px;"&gt;                   
+These investments did not alter the achievement of the environmental or social characteristics promoted by the Sub-Fund, and their purpose was investment, contributing to efficient portfolio management, providing liquidity and hedging.&lt;/p&gt;
+&lt;p style="margin-top: -10px;"&gt; The Investment Manager has established minimum environmental or social safeguards so as not to cause significant damage, such as consideration of the principal adverse impacts, or the exclusion of activities that are not aligned with the environmental and/or social characteristics of the Fund. The assets that could be considered were the following:&lt;/p&gt;
+&lt;ul&gt;
+                    &lt;li&gt;Direct cash investment assets that did not have an ESG rating/rating due to the lack of supplier data used by the Investment Manager and which cannot be considered sustainable investments in accordance with the criterion defined in the previous section (i.e., green, social bonds, etc.).&lt;/li&gt;
+                    &lt;li&gt;Investment funds that did not have an ESG rating/rating due to lack of data and that cannot be classified as an investment Sub-Fund art. 8 or 9 according to SFDR.&lt;/li&gt;
+                    &lt;li&gt;Other cash assets other than those mentioned above. (i.e., ETC, etc.) that are permitted by the Sub-Fund's policy and do not harm its ESG profile.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
   </si>
 </sst>
 </file>
@@ -3976,10 +3972,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2CF707-1372-4610-A1C4-0399A26E6B10}">
   <dimension ref="A1:CY18"/>
   <sheetViews>
-    <sheetView topLeftCell="CL1" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="BZ1" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="CN2" sqref="CN2"/>
+      <selection pane="bottomLeft" activeCell="CC1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4333,7 +4329,7 @@
         <v>232</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>211</v>
@@ -4351,7 +4347,7 @@
         <v>339</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>331</v>
@@ -4366,7 +4362,7 @@
         <v>335</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>145</v>
@@ -4375,7 +4371,7 @@
         <v>76</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>233</v>
@@ -4399,7 +4395,7 @@
         <v>237</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AI2" s="2" t="s">
         <v>238</v>
@@ -4528,7 +4524,7 @@
         <v>214</v>
       </c>
       <c r="BY2" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="BZ2" s="2" t="s">
         <v>291</v>
@@ -4582,7 +4578,7 @@
         <v>312</v>
       </c>
       <c r="CQ2" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="CR2" s="2" t="s">
         <v>313</v>
@@ -4644,7 +4640,7 @@
         <v>232</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>211</v>
@@ -4662,7 +4658,7 @@
         <v>339</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>331</v>
@@ -4955,7 +4951,7 @@
         <v>232</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>211</v>
@@ -4973,7 +4969,7 @@
         <v>339</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>331</v>
@@ -5266,7 +5262,7 @@
         <v>232</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>211</v>
@@ -5284,7 +5280,7 @@
         <v>339</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>331</v>
@@ -5577,7 +5573,7 @@
         <v>232</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>211</v>
@@ -5595,7 +5591,7 @@
         <v>339</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>331</v>
@@ -5888,7 +5884,7 @@
         <v>232</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>211</v>
@@ -5906,7 +5902,7 @@
         <v>339</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>331</v>
@@ -6199,7 +6195,7 @@
         <v>232</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>211</v>
@@ -6217,7 +6213,7 @@
         <v>339</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>331</v>
@@ -6510,7 +6506,7 @@
         <v>232</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>211</v>
@@ -6528,7 +6524,7 @@
         <v>339</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>331</v>
@@ -6821,7 +6817,7 @@
         <v>232</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>211</v>
@@ -6839,7 +6835,7 @@
         <v>339</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>331</v>
@@ -7132,7 +7128,7 @@
         <v>232</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>211</v>
@@ -7150,7 +7146,7 @@
         <v>339</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>331</v>
@@ -7443,7 +7439,7 @@
         <v>232</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>211</v>
@@ -7461,7 +7457,7 @@
         <v>339</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S12" s="2" t="s">
         <v>331</v>
@@ -7754,7 +7750,7 @@
         <v>232</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>211</v>
@@ -7772,7 +7768,7 @@
         <v>339</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>331</v>
@@ -8065,7 +8061,7 @@
         <v>232</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>211</v>
@@ -8083,7 +8079,7 @@
         <v>339</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>331</v>
@@ -8376,7 +8372,7 @@
         <v>232</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>211</v>
@@ -8394,7 +8390,7 @@
         <v>339</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>331</v>
@@ -8687,7 +8683,7 @@
         <v>232</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>211</v>
@@ -8705,7 +8701,7 @@
         <v>339</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>331</v>
@@ -8998,7 +8994,7 @@
         <v>232</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>211</v>
@@ -9016,7 +9012,7 @@
         <v>339</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>331</v>
@@ -9288,9 +9284,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6A6837-7230-4429-B7FC-980D5EFB5D43}">
   <dimension ref="A1:CY17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="BZ1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CA1" sqref="A1:XFD2"/>
+      <selection pane="bottomLeft" activeCell="CC1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10137,10 +10133,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF83BCF-3DAB-4382-89FD-168493B9C498}">
   <dimension ref="A1:CY3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BU1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="CH1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="BO1" sqref="BO1"/>
-      <selection pane="bottomLeft" activeCell="BY1" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="CL2" sqref="CL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10503,7 +10499,7 @@
         <v>215</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>382</v>
@@ -10512,7 +10508,7 @@
         <v>383</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="S2" s="18" t="s">
         <v>384</v>
@@ -10536,7 +10532,7 @@
         <v>389</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>390</v>
@@ -10548,58 +10544,58 @@
         <v>392</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>393</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>394</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="AI2" s="2" t="s">
         <v>395</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>396</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="AM2" s="2" t="s">
         <v>397</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="AP2" s="2" t="s">
         <v>398</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>399</v>
       </c>
       <c r="AS2" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="AT2" s="2" t="s">
         <v>400</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="AV2" s="2" t="s">
         <v>401</v>
@@ -10614,7 +10610,7 @@
         <v>404</v>
       </c>
       <c r="AZ2" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="BA2" s="2" t="s">
         <v>405</v>
@@ -10657,16 +10653,16 @@
       </c>
       <c r="BN2" s="2"/>
       <c r="BO2" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="BP2" s="2" t="s">
         <v>418</v>
       </c>
       <c r="BQ2" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="BR2" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="BS2" s="2" t="s">
         <v>419</v>
@@ -10699,73 +10695,73 @@
         <v>426</v>
       </c>
       <c r="CC2" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="CD2" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="CD2" s="2" t="s">
+      <c r="CE2" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="CF2" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="CE2" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="CF2" s="2" t="s">
+      <c r="CG2" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="CG2" s="2" t="s">
+      <c r="CH2" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="CH2" s="2" t="s">
+      <c r="CI2" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="CI2" s="2" t="s">
+      <c r="CJ2" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="CJ2" s="2" t="s">
+      <c r="CK2" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="CK2" s="2" t="s">
+      <c r="CL2" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="CM2" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="CL2" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="CM2" s="2" t="s">
+      <c r="CN2" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="CO2" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="CN2" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="CO2" s="2" t="s">
+      <c r="CP2" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="CQ2" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="CP2" s="2" t="s">
+      <c r="CR2" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="CQ2" s="2" t="s">
+      <c r="CS2" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="CT2" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="CR2" s="2" t="s">
+      <c r="CU2" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="CV2" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="CS2" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="CT2" s="2" t="s">
+      <c r="CW2" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="CX2" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="CU2" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="CV2" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="CW2" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="CX2" s="2" t="s">
-        <v>442</v>
-      </c>
       <c r="CY2" s="2" t="s">
-        <v>437</v>
+        <v>559</v>
       </c>
     </row>
     <row r="3" spans="1:103" ht="171" customHeight="1" x14ac:dyDescent="0.35">
@@ -10812,7 +10808,7 @@
         <v>215</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="P3" s="18" t="s">
         <v>382</v>
@@ -10821,7 +10817,7 @@
         <v>383</v>
       </c>
       <c r="R3" s="18" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="S3" s="18" t="s">
         <v>384</v>
@@ -10845,7 +10841,7 @@
         <v>389</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="AA3" s="2" t="s">
         <v>390</v>
@@ -10857,58 +10853,58 @@
         <v>392</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="AE3" s="2" t="s">
         <v>393</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="AG3" s="2" t="s">
         <v>394</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="AI3" s="2" t="s">
         <v>395</v>
       </c>
       <c r="AJ3" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>396</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="AM3" s="2" t="s">
         <v>397</v>
       </c>
       <c r="AN3" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="AP3" s="2" t="s">
         <v>398</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="AR3" s="2" t="s">
         <v>399</v>
       </c>
       <c r="AS3" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="AT3" s="2" t="s">
         <v>400</v>
       </c>
       <c r="AU3" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="AV3" s="2" t="s">
         <v>401</v>
@@ -10923,7 +10919,7 @@
         <v>404</v>
       </c>
       <c r="AZ3" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="BA3" s="2" t="s">
         <v>405</v>
@@ -10966,16 +10962,16 @@
       </c>
       <c r="BN3" s="2"/>
       <c r="BO3" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="BP3" s="2" t="s">
         <v>418</v>
       </c>
       <c r="BQ3" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="BR3" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="BS3" s="2" t="s">
         <v>419</v>
@@ -11008,73 +11004,73 @@
         <v>426</v>
       </c>
       <c r="CC3" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="CD3" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="CD3" s="2" t="s">
+      <c r="CE3" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="CF3" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="CE3" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="CF3" s="2" t="s">
+      <c r="CG3" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="CG3" s="2" t="s">
+      <c r="CH3" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="CH3" s="2" t="s">
+      <c r="CI3" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="CI3" s="2" t="s">
+      <c r="CJ3" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="CJ3" s="2" t="s">
+      <c r="CK3" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="CK3" s="2" t="s">
+      <c r="CL3" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="CM3" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="CL3" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="CM3" s="2" t="s">
+      <c r="CN3" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="CO3" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="CN3" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="CO3" s="2" t="s">
+      <c r="CP3" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="CQ3" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="CP3" s="2" t="s">
+      <c r="CR3" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="CQ3" s="2" t="s">
+      <c r="CS3" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="CT3" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="CR3" s="2" t="s">
+      <c r="CU3" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="CV3" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="CS3" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="CT3" s="2" t="s">
+      <c r="CW3" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="CX3" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="CU3" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="CV3" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="CW3" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="CX3" s="2" t="s">
-        <v>442</v>
-      </c>
       <c r="CY3" s="2" t="s">
-        <v>437</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -11086,17 +11082,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F6EF4D-CF5F-40A8-8775-A1A29C91F1C4}">
   <dimension ref="A1:DA3"/>
   <sheetViews>
-    <sheetView topLeftCell="BU1" workbookViewId="0">
+    <sheetView topLeftCell="BY1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="CA1" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="CE1" sqref="CE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="29" width="19.36328125" customWidth="1"/>
     <col min="30" max="30" width="42.54296875" customWidth="1"/>
-    <col min="31" max="105" width="19.36328125" customWidth="1"/>
+    <col min="31" max="82" width="19.36328125" customWidth="1"/>
+    <col min="83" max="83" width="63.54296875" customWidth="1"/>
+    <col min="84" max="105" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:105" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -11424,16 +11422,16 @@
         <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>142</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>141</v>
@@ -11442,292 +11440,292 @@
         <v>75</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="19" t="s">
+        <v>546</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="O2" s="19" t="s">
-        <v>551</v>
-      </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="U2" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>461</v>
-      </c>
       <c r="W2" s="2" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>145</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="AG2" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="AK2" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="AO2" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="AG2" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="AU2" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="AM2" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="AW2" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="AO2" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AY2" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="AU2" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="AW2" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="AX2" s="2" t="s">
+      <c r="BA2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="AY2" s="2" t="s">
+      <c r="BB2" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="BC2" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="AZ2" s="2" t="s">
+      <c r="BD2" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="BA2" s="2" t="s">
+      <c r="BE2" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="BB2" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="BC2" s="2" t="s">
+      <c r="BF2" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="BD2" s="2" t="s">
+      <c r="BG2" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="BE2" s="2" t="s">
+      <c r="BH2" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="BF2" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="BG2" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="BI2" s="2" t="s">
         <v>411</v>
       </c>
       <c r="BJ2" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="BM2" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="BK2" s="2" t="s">
+      <c r="BN2" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="BL2" s="2" t="s">
+      <c r="BO2" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="BM2" s="2" t="s">
+      <c r="BP2" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="BN2" s="2" t="s">
+      <c r="BQ2" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="BR2" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="BO2" s="2" t="s">
+      <c r="BS2" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="BV2" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="BP2" s="2" t="s">
+      <c r="BW2" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="BY2" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="BQ2" s="2" t="s">
+      <c r="BZ2" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="CA2" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="CB2" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="CC2" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="CD2" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="CE2" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="CF2" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="CG2" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="BR2" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="BS2" s="2" t="s">
+      <c r="CH2" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="CI2" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="CJ2" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="CK2" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="CL2" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="CM2" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="CN2" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="BT2" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="BU2" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="BV2" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="BW2" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="BX2" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="BY2" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="BZ2" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="CA2" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="CB2" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="CC2" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="CD2" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="CE2" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="CF2" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="CG2" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="CH2" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="CI2" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="CJ2" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="CK2" s="2" t="s">
+      <c r="CO2" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="CL2" s="2" t="s">
+      <c r="CP2" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="CQ2" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="CM2" s="2" t="s">
+      <c r="CR2" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="CN2" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="CO2" s="2" t="s">
+      <c r="CS2" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="CP2" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="CQ2" s="2" t="s">
+      <c r="CT2" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="CR2" s="2" t="s">
+      <c r="CU2" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="CS2" s="2" t="s">
+      <c r="CV2" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="CT2" s="2" t="s">
+      <c r="CW2" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="CX2" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="CU2" s="2" t="s">
+      <c r="CY2" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="CZ2" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="CV2" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="CW2" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="CX2" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="CY2" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="CZ2" s="2" t="s">
-        <v>513</v>
-      </c>
       <c r="DA2" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="3" spans="1:105" s="2" customFormat="1" ht="197" customHeight="1" x14ac:dyDescent="0.35">
@@ -11738,16 +11736,16 @@
         <v>134</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>142</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>141</v>
@@ -11756,292 +11754,292 @@
         <v>75</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="19" t="s">
+        <v>546</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="O3" s="19" t="s">
-        <v>551</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="U3" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>461</v>
-      </c>
       <c r="W3" s="2" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>145</v>
       </c>
       <c r="Y3" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="AC3" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="Z3" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="AG3" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="AI3" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="AK3" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="AD3" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="AO3" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="AG3" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="AK3" s="2" t="s">
+      <c r="AR3" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AS3" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="AU3" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="AM3" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="AN3" s="2" t="s">
+      <c r="AV3" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="AW3" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="AO3" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="AP3" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="AQ3" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="AR3" s="2" t="s">
+      <c r="AX3" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="AS3" s="2" t="s">
+      <c r="AY3" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="AU3" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="AV3" s="2" t="s">
+      <c r="AZ3" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="AW3" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="AX3" s="2" t="s">
+      <c r="BA3" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="AY3" s="2" t="s">
+      <c r="BB3" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="BC3" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="AZ3" s="2" t="s">
+      <c r="BD3" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="BA3" s="2" t="s">
+      <c r="BE3" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="BB3" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="BC3" s="2" t="s">
+      <c r="BF3" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="BD3" s="2" t="s">
+      <c r="BG3" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="BE3" s="2" t="s">
+      <c r="BH3" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="BF3" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="BG3" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="BH3" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="BI3" s="2" t="s">
         <v>411</v>
       </c>
       <c r="BJ3" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="BK3" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="BL3" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="BM3" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="BK3" s="2" t="s">
+      <c r="BN3" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="BL3" s="2" t="s">
+      <c r="BO3" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="BM3" s="2" t="s">
+      <c r="BP3" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="BN3" s="2" t="s">
+      <c r="BQ3" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="BR3" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="BO3" s="2" t="s">
+      <c r="BS3" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="BT3" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="BU3" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="BV3" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="BP3" s="2" t="s">
+      <c r="BW3" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="BX3" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="BY3" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="BQ3" s="2" t="s">
+      <c r="BZ3" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="CA3" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="CB3" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="CC3" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="CD3" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="CE3" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="CF3" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="CG3" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="BR3" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="BS3" s="2" t="s">
+      <c r="CH3" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="CI3" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="CJ3" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="CK3" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="CL3" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="CM3" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="CN3" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="BT3" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="BU3" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="BV3" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="BW3" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="BX3" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="BY3" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="BZ3" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="CA3" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="CB3" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="CC3" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="CD3" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="CE3" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="CF3" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="CG3" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="CH3" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="CI3" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="CJ3" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="CK3" s="2" t="s">
+      <c r="CO3" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="CL3" s="2" t="s">
+      <c r="CP3" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="CQ3" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="CM3" s="2" t="s">
+      <c r="CR3" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="CN3" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="CO3" s="2" t="s">
+      <c r="CS3" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="CP3" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="CQ3" s="2" t="s">
+      <c r="CT3" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="CR3" s="2" t="s">
+      <c r="CU3" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="CS3" s="2" t="s">
+      <c r="CV3" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="CT3" s="2" t="s">
+      <c r="CW3" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="CX3" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="CU3" s="2" t="s">
+      <c r="CY3" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="CZ3" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="CV3" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="CW3" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="CX3" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="CY3" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="CZ3" s="2" t="s">
-        <v>513</v>
-      </c>
       <c r="DA3" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated narrative table to  fix one link that was wrong
</commit_message>
<xml_diff>
--- a/excel_books/narratives_tables.xlsx
+++ b/excel_books/narratives_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://santandernet.sharepoint.com/sites/ESGTEAM552/Shared Documents/Archivos/Archivos Red/Fondos éticos/09. REGULACIÓN/04_SFDR/Info_Periódica/Revisión_generación/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{04296667-9EFD-44F9-BBA6-B3E6F222A1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAD612AF-039B-477E-BC96-BC113E05058D}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="8_{04296667-9EFD-44F9-BBA6-B3E6F222A1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3602844D-3BF0-46D0-8716-BE8A9BAB7086}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="3" xr2:uid="{876AE5F7-9A61-4241-A259-03591D994349}"/>
   </bookViews>
@@ -3476,17 +3476,11 @@
 &lt;p&gt;Neste caso, a Sociedade Gestora estabeleceu procedimentos para verificar se esses instrumentos não alteram a concretização das caraterísticas ambientais ou sociais promovidas pelo Fundo de Pensões, e esses instrumentos podem ser utilizados para efeitos de cobertura e gestão eficiente da carteira do Fundo de Pensões de Investimento como elemento de diversificação e gestão.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>art8_feeder_noprev_pt</t>
-  </si>
-  <si>
-    <t>Não aplicável, porque não existe um período de referência anterior</t>
-  </si>
-  <si>
     <t>&lt;p&gt;
-Durante o período de referência, foram tomadas as seguintes medidas para cumprir com as características ambientais e sociais do Fundo:
+Durante o período de referência, foram tomadas as seguintes medidas para cumprir com as características ambientais e sociais do  Fundo de Pensões:
 &lt;/p&gt;
 &lt;ul&gt;
-  &lt;li&gt;A Sociedade Gestora verificou periodicamente se o Fundo cumpre as seguintes exclusões:
+  &lt;li&gt;A Sociedade Gestora verificou periodicamente se o  Fundo de Pensões cumpre as seguintes exclusões:
     &lt;ul&gt;
       &lt;li&gt;Foram excluídos os emitentes com exposição (medida em termos de volume de negócios) relacionada com armas controversas e/ou com exposição significativa a combustíveis fósseis não convencionais e/ou atividades de produção de energia a partir carvão e/ou da extração de carvão.
       &lt;/li&gt;
@@ -3517,6 +3511,12 @@
   &lt;p&gt; https://www.santanderassetmanagement.pt/santander-pensoes/informacao-corporativa-santander-pensoes
   &lt;/p&gt;
 &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>art8_feeder_noprev_pt</t>
+  </si>
+  <si>
+    <t>Não aplicável, porque não existe um período de referência anterior</t>
   </si>
 </sst>
 </file>
@@ -11290,8 +11290,8 @@
   <dimension ref="A1:DA5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="AM2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AQ6" sqref="AQ6"/>
+      <pane ySplit="1" topLeftCell="CE3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CP4" sqref="CP4"/>
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -12527,7 +12527,7 @@
         <v>550</v>
       </c>
       <c r="CP4" s="2" t="s">
-        <v>551</v>
+        <v>580</v>
       </c>
       <c r="CQ4" s="12" t="s">
         <v>552</v>
@@ -12568,7 +12568,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>469</v>
@@ -12658,7 +12658,7 @@
         <v>492</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="AG5" s="12" t="s">
         <v>494</v>
@@ -12814,7 +12814,7 @@
         <v>541</v>
       </c>
       <c r="CG5" s="2" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="CH5" s="12" t="s">
         <v>543</v>
@@ -12841,7 +12841,7 @@
         <v>550</v>
       </c>
       <c r="CP5" s="2" t="s">
-        <v>582</v>
+        <v>551</v>
       </c>
       <c r="CQ5" s="12" t="s">
         <v>552</v>
@@ -12884,6 +12884,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee51a08e-cffb-442e-9a85-1980beacc2f8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9f04ef3f-090d-46e3-96be-1fbea4829461" xsi:nil="true"/>
+    <Comment xmlns="ee51a08e-cffb-442e-9a85-1980beacc2f8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EA6A4DE027E6E4386DF60BFAE3B87E5" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3abf4d3fcc761b62f1df79a5388292c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee51a08e-cffb-442e-9a85-1980beacc2f8" xmlns:ns3="9f04ef3f-090d-46e3-96be-1fbea4829461" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="352dc0540605a416d022d0321880f487" ns2:_="" ns3:_="">
     <xsd:import namespace="ee51a08e-cffb-442e-9a85-1980beacc2f8"/>
@@ -13098,29 +13119,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee51a08e-cffb-442e-9a85-1980beacc2f8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9f04ef3f-090d-46e3-96be-1fbea4829461" xsi:nil="true"/>
-    <Comment xmlns="ee51a08e-cffb-442e-9a85-1980beacc2f8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9745F6CE-11AD-4547-BE02-8622392B4837}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5FDC5C-D626-4B87-97B5-B79DFC26F2FE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13128,5 +13128,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5FDC5C-D626-4B87-97B5-B79DFC26F2FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9745F6CE-11AD-4547-BE02-8622392B4837}"/>
 </file>
</xml_diff>